<commit_message>
Get daily reddit data: Tue Jun  3 08:13:36 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_08.xlsx
+++ b/data/collected_data/2025_06_08.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C524"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3797 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1l24quh</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Beginner nail drill recommendations?</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l24quh/beginner_nail_drill_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1l255c9</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>I am obsessed 🌸😍🎀</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l255c9</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1l24z5w</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Which shape?</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l24z5w</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1l24007</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>first time in square 🥹</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ch8ljhn4fn4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1l23zhj</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>embarrassed/nervous</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9hppf57vdn4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1l23rns</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Should I keep them, trim them, or wing it?</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l23rns</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1l21crh</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>How to tell when you don't need to cut the PNF?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l21crh</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1l21r6v</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>4 weeks of chrome! No chips!</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9udpvbvzrm4f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1l1yk7x</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Don’t be Koi about it 🎏✨</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1yk7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1l1wm2j</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Shape</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rdrvtimkil4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1l1u4bg</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Nail machine malfunction</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l1u4bg/nail_machine_malfunction/</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1l1toqg</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Nails Won’t Stop Chipping</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvdkjiphwk4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1l1t8nq</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Nail tear a week before my birthday, would it still be safe to put on a set?</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rk5kvz5ftk4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1l1t4ix</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Nails I had for my 8 year anniversary!</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1t4ix</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1l1syau</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>what am i doing wrong?</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l1syau/what_am_i_doing_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1l1xkec</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Learning to do my own nails after these disasters</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1xkec</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1l1yg9f</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>nail lady delivered ❤️</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jvz5h441yl4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1l1y5dy</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>trans pride french tips</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1y5dy</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1l1yvnt</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>My Kendrick Lamar GNX album inspired mani worn to his 5/29 SF show (swipe to see some of my inspo and mock up)</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1yvnt</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1l233rs</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Skull Panda inspired look I tried out ☺️</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l233rs</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1l23isy</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>How do I get creative nails?</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l23isy/how_do_i_get_creative_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1l2382y</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>#nails</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/liyas.lovely.nails?igsh=eDkxaGY3Z2htbWRz</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1l21m66</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Shellac on a 5 year old</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l21m66/shellac_on_a_5_year_old/</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1l235q3</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Clear acrylic tips that don't need builder?</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l235q3/clear_acrylic_tips_that_dont_need_builder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1l21zzz</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Prom nails</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l21zzz</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1l233vg</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Skull Panda inspired look I tried out!</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l233vg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1l22w8k</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Is this considered normal or fast nail growth at 3 weeks? (Before and after).</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l22w8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1l21wni</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Pride</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5eadb4ghtm4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1l21q18</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>I cut the tip of my finger a day before my nail appt :c</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l21q18</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1l21pvt</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Nail tech tingz</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0z2ns4ymrm4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1l21mqu</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Rhapsody in Blue 💙💜</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l21mqu</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1l1zvl6</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Subtle glitter 💅🏻</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nq21h3ypam4f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1l1xezx</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>weird line</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6lfknch3pl4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1l21iwh</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Not perf, but so shiny!!</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l21iwh</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1l20pna</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Inspired by u/tinkleblades !</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bwd0mlnbim4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1l214cl</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Beautiful nails</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l214cl</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1l2125y</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>my new set for grad 😛</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2125y</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1l2104f</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>is this a normal thickness?</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wrzh0bhxkm4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1l20tjp</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>All the nails I’ve done within the past few months!</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l20tjp</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1l20qqr</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Tried to add a snake</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m4r1tq2mim4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1l20d1t</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Color I got vs the one I asked for</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l20d1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1l1zvkr</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Attempted a 3D flower</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1zvkr</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1l1zrkx</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>How did I do?</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1zrkx</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1l1zc6g</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Vacay nails! 🌺</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1738vux5m4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1l1zb0i</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>I am loving this color to start the summer!</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1zb0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1l1ytcj</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>I loved the result.</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/spcxevh91m4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1l1yqiq</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Vegas themed nails!</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ucho40sj0m4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1l1yobc</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Flower power</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3ezn1kzzl4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1l1y5j4</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Gucci - Dorothy Turquoise</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1y5j4</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1l1y3l9</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Fuzzy rainbow nails to kick off pride month🌈✨💅🏼</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jmqypg2yul4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1l1xnxq</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Love getting my nails</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1xnxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1l1xi7r</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>My FAVORITE Cat Eye 😻</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1xi7r</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1l1x888</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>so obsessed 🌸</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1x888</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1l1x1ww</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Something bright for summer</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xkhovl53ml4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1l1wp4m</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Nails match my coffee cup 🥰</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zpifdrt8jl4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1l1wd91</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>my very first time doing french tips</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1wd91</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1l1vzhr</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Yay or Nay?</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pg04huhldl4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1l1vui2</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Long hair baddies.. helppp</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f7ofh9uhcl4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1l1vtjb</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>I love this so muchh</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqsw94n9cl4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1l1vo5m</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>beeeeeeeeeeeeees</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1vo5m</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1l1vnt7</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Am I being crazy for not liking my nails?</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1vnt7</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1l1vn3s</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>citrus ♡</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1vn3s</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1l1vmjq</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>mermaid themed, thoughts?</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1vmjq</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1l1vkbc</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Icy queen!</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1vkbc</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1l1vebo</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Bf proposed with perfect timing</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1vebo</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1l1v9my</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>I want your honest opinion about my nails - what can I improve? I oil them every day and have 3 weeks of regrowth but I have to go to my nail specialist in 4 days. Please be honest!</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1v9my</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1l1v9e8</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Summer fun</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/flrkcj808l4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1l1v7td</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Evil eye nails on the W train in NYC. 🧿❤️</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fu6fvifo7l4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1l1uxzv</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>My nails today 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qcdeczxn5l4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1l1uvat</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Nails I did</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l1uvat/nails_i_did/</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1l1us3k</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Is it just me or is this a bad gel application?</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1us3k</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1l1ujdl</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>just did this press on set and it matches her earrings so well!</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1ujdl</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1l1tra7</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>I hate my nail colour</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1tra7</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1l1tc5z</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Any techs/salons in NYC that can do nail art like this?</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1tc5z</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1l1t95q</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>bad nails</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ns5p7jvktk4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1l1t74z</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>My nails for my friends wedding</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1t74z</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1l1t2p9</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Is something off or am I just not used to nails</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1t2p9</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1l1sfbn</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Am I just not meant to get my nails done?</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/55nruipunk4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1l1svfv</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>It’s that time of year 🏳️‍🌈 💅</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1svfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1l1slo5</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>First time getting short acrylics</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1slo5</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1l1rzzs</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>first-time getting my nails done, do I need to visit the nail salon to cut my grown nails?</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1rzzs</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1l1rkzz</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>continuing gel nail hobby after learning I may have a higher risk of skin cancer</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l1rkzz/continuing_gel_nail_hobby_after_learning_i_may/</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1l1rvk7</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Subtle pride nails 🩷💜💙</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1rvk7</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1l1rnxw</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Question about acyrlic nails</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l1rnxw/question_about_acyrlic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1l1rn2u</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>I managed to remove biab without damaging my nails!</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1rn2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1l1rhdb</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>diy nails</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1rhdb</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1l1r98y</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>What do you think? Aren't they too cheesy?</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sb7xyr5nfk4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1l1qs7y</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Is there any hope for this nail?</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1qs7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1l1qs2k</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>[Credit richklaws on insta] what service am I looking for?</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/36h8vi3dck4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1l1qowu</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Air bubbles.</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1qowu</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1l1qnea</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Daughter got acrylics at 6 years old</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l1qnea/daughter_got_acrylics_at_6_years_old/</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1l1qm7d</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Unicorn Mermaid Pride</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1qm7d</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1l1q2uc</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>look at my favourite nails i did on my self ☺️</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0o10b6xk7k4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1l1q2j1</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>My Super Cute Nails ^_^</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y999h8aa7k4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1l1pwvs</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Glossy blue for a rainy day</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q5brkbif6k4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1l1ppz9</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Night Armor 🌙✨</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/19311ztk4k4f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1l1p8pf</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Happy pride month!</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f75mi41v1k4f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1l1ou0o</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Baby pink gel on natural nails. My nail artist always kills it on shaping IMO</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pobbf7x6zj4f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1l1e0dt</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>I’m expecting itchiness around my cuticles:(</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l1e0dt/im_expecting_itchiness_around_my_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1l1ii1a</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>How do I get my nails done and painted like this? Do I just go into any salon and ask for it or do I need to find an artist in my area?</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1ii1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1l25m6y</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Hot pink lift</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cq63t5owxn4f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1l24lf0</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>12/10 Customer Service experience</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l24lf0/1210_customer_service_experience/</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1l24c0x</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Pretty in pink</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fplv1vfwin4f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1l243h7</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Nails from May :)</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l243h7</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1l23ja6</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>I love a fun magnetic polish + topper combo</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l23ja6</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1l237u9</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Help with bridesmaid nails!!</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l237u9/help_with_bridesmaid_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1l23fzd</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>“Soap” &amp; Glitter</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l23fzd</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1l23cum</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>nothing I love more than a classic Barbie pink manicure</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ik5trnk58n4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1l23cdg</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>mooncat’s star destroyer in other colors?</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l23cdg/mooncats_star_destroyer_in_other_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1l22fhz</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Pride Nails 🌈</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l22fhz</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1l21ncx</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>First set of June!</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l21klt</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1l2112k</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Do you have a “signature color”?</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l2112k/do_you_have_a_signature_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1l20k1b</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Zoya Perfectors ❤️</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yuhltv8vgm4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1l2011n</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>My Cup Runneth Over</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2011n</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1l1zxzo</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Tips for working with Maniology aqua topper (or alternative recs)?</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j0tyg0nbbm4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1l1zrbb</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Oh Splat</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1zrbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1l1z5dn</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>This got to be my prettiest drug store polish ever</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3pzthid84m4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1l1z1lc</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>🪐Saturn’s Ring☄️</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1z1lc</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1l1ysjn</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Nail polish remover recs?</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l1ysjn/nail_polish_remover_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1l1ys2g</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>What I wore in May</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1ys2g</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1l1y814</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Distracted by my nails</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1xaw4</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1l1xluh</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Yo, listen up here's a story About a little guy That lives in a blue world</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1xluh</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1l1y37o</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>any polishes that look like an actual melonberry?</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tsbkmtluul4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1l1y1tk</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>An apology done right</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l1y1tk/an_apology_done_right/</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1l1y1hm</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>dupe for jump jump bug?</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqcd099gul4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1l1xnyk</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Never Tide Down 💙🩵🌊</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rxt7qhnytk4f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1l1xf7o</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Looking for more like DMD</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aroj1s85pl4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1l1x8r9</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Neon pink</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pzgov0bonl4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1l1x2p1</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Big Monster Energy (Drink)</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1x2p1</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1l1w37j</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>KBShimmer- One in a Melon 💖</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1w37j</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1l1vi4i</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>A Talent for Misfortune</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1vi4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1l1uuim</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>In My Element🤍🩵</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1uuim</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1l1ufxs</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>National Polish Day Mani</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5t1iddry1l4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1l1u745</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Nails and mugs</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nxb0fvo60l4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1l1u4ag</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Mani today</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1u4ag</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1l1tr4u</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>When the sun hits just right for the rainbow to flash</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wldjzz43xk4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1l1to8t</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Switch Nails</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1to8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1l1teis</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>D e l i r i u m</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ga9r7akuk4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1l1tavw</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>My nails look so magical</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/93l786hutk4f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1l1t70d</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>persimmon/tomato nails!</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dv6aed06tk4f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1l1t34z</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Short and sweet 🍬</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1t34z</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1l1svls</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Monthly Mani Challenge Megathread 🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcn1y845qk4f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1l1srue</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Teal + holo</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvt3pu89qk4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1l1shhq</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Fairy shimmer tie dye!</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1shhq</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1l1s7xr</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Happy Pride ❤️🧡💛💚💙💜</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r47tuebfmk4f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1l1s04a</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Such a fun neutral!</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1s04a</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1l1rryd</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>3D effect</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p5der31ajk4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1l1rf0b</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Fragrance free nail help!</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l1rf0b/fragrance_free_nail_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1l1r7ik</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>A little spacey a little oceany</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1r7ik</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1l1r0y4</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>everything is blooming! 🌺</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1r0y4</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1l1qyyl</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Subtle pride nails!!</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/piqolc9ndk4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1l1qy7z</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Similar to Vishine "Hot Rose Pink" but not gel?</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l1qy7z/similar_to_vishine_hot_rose_pink_but_not_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1l1qo1g</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Duped myself 4x</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1qo1g</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1l1q7fb</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Nail Polish in the UK (London)</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l1q7fb/nail_polish_in_the_uk_london/</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1l1q6qp</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>help me pick my graduation polish!</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l1q6qp/help_me_pick_my_graduation_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1l1pj62</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>non-gel recommendations for something like this?</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4q19kdwt3k4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1l1p9b5</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>define "palate cleanser"</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1p9b5</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1l1p6dz</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Maelstrom/Mermaid Bait Combo</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1p6dz</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1l1p5id</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Pride mani</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g14xd6s91k4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1l1p4pr</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Felt like something soft and ethereal this week ✨</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1p4pr</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1l1p43e</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Do biodegradable glitters work in polishes?</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l1p43e/do_biodegradable_glitters_work_in_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1l1p1dq</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>What’s your go-to crème under House of Hades?</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l1p1dq/whats_your_goto_crème_under_house_of_hades/</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1l1p196</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Space Oddity</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1p196</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1l1oz5b</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Fancy Gloss magnets</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czwhutq30k4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1l1otrs</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Polished For Days literally never misses</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1otrs</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1l1idku</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Best Pink and gree/yellow Neons this season</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l1idku/best_pink_and_greeyellow_neons_this_season/</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1l1izcl</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>BKL Kikimora dupe??</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfo9liacui4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1l1obka</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Grieve w me</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rs4ekrovj4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1l1nxk3</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Indie shimmers: reddish-pink comparison</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1nxk3</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1l1nv31</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Becoming a fan of reds</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1nv31</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1l1nfv9</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>White primer recommendations?</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1nfv9</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1l1nfnt</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>🏳️‍🌈🌈happy pride! 🌈🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1nfnt</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1l1myz5</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Nails Need Rehab</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1myz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1l1m0r7</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>This color reminds me of 90’s clear blow up furniture! I’m obsessed. Mooncat: Poems For A Harvest Moon.</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1m0r7</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1l1la2d</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>this literally happens EVERY time whenever I’ve to attend an event the next day or so</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/28o861gkaj4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1l1kuqj</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>It's empty!</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/di4l3qtk7j4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1l1kn80</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>To say I'm obsessed is an understatement</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1kn80</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1l1klzq</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>You Know Her, You Love Her, You Hate Her Formula</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kf6ul8qu5j4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1l1kihw</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>What is going on here?</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1kihw</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1l1kg0n</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Pride nails but for someone that doesn't wear bright colors</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1kg0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1l1jkvl</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Pastel Pride 🌈✨</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1jkvl</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1l1ind5</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Slythery little snake 🐍</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1ind5</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1l1icx9</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Pride nails ft. Cat Tax🩷💜💙</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1icx9</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1l1iajq</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Rocking some pride nails on my new shorties 🌈</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6nvixmo1pi4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1l1i9n7</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>If you could only choose ONE nail color to wear for the rest of your life, what would it be?</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>/r/Nails/comments/1l10fuv/if_you_could_only_choose_one_nail_color_to_wear/</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1l1hulb</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Togepi frenchies 💙❤️</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1hulb</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1l1hpfa</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>My Canadian polish mani 🍁</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g88hw5egki4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1l1hghc</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>1st time with a dotting tool - oof!</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1hghc</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1l1h94l</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>My Pansexual Pride Nails</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2onbpntgi4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1l1h5cs</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Did my nails to match my dress</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1h5cs</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1l1h3k8</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Landlord special, magnetic edition</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1h3k8</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1l1gapd</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Happy prideee</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1gapd</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1l10puu</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Pure ice nail polish</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ul8ue1ttxd4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1l14oaj</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Gel allergy question</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l14oaj/gel_allergy_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1l1fww0</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Mooncat soft glowy pinks</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1fww0</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1l1f09k</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>🖤🩶🤍💜🌌</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r2nblktyvh4f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1l1e86g</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Newbie nails</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j07zaj5knh4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1l1e44o</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l1e44o/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1l1dx5f</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Getting back into painting my nails - in love with this polish!</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1dx5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1l1dtiw</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Skin undertone and lacquer colors</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l1dtiw/skin_undertone_and_lacquer_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1l23h9p</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Any ideas?</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l23h9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1l23h70</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Gothic music festival flair</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l23h70</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1l21tmv</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>first nail art set 💗</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l21tmv</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1l21qvb</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>extra large 💅</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l21qvb</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1l216yz</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>first time doing gel x on someone else!</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vgk5vdvmmm4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1l206q7</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Pride set ❤️🧡💛</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l206q7</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1l1zedc</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Pride set done by me</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r5wz5w5h6m4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1l1z98z</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Happy Pride 🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1z98z</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1l1y57y</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Pride nails 🏳️‍🌈✨🪩</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1y57y</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1l1y1d3</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>What should my next set be?</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1l1y1d3/what_should_my_next_set_be/</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1l1xzn5</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>wedding nails</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5682c170ul4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1l1xjrb</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Camo Inspo</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1xjrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1l1womd</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>New nails look like candy!</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cj5qg3v4jl4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1l1vj2y</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Here’s my attempt at Pride month nails! ❤️🧡💛💚💙💜</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1vj2y</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1l1usrq</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Super fun for summer 💅💛</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/314newel4l4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1l1tw2p</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Porcelain &amp; Lemons 🍋</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zh0yl812yk4f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1l1sd7o</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>The deer keep eating our tomato plants so I’m taking the matter into my own hands</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1sd7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1l1phcc</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Night Armor 🌙✨</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/opl8vdct2k4f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1l1oxs5</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Pink Lemonade &amp; Flowers</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1oxs5</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1l1nm86</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>pomegranate red star accent nails 💫</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oypif0msqj4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1l1niwg</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>blue floral accent nail</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1niwg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1l1lscr</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>What is the best brand for Nail tips/ press on nails you can paint yourself?</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1l1lscr/what_is_the_best_brand_for_nail_tips_press_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1l1gw5j</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Design my nails?! Pleaseee x</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l1gw5j</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jun  4 08:13:08 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_08.xlsx
+++ b/data/collected_data/2025_06_08.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C524"/>
+  <dimension ref="A1:C721"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9341,6 +9341,3355 @@
         </is>
       </c>
     </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1l2xvnx</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Press on feeling…</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l2xvnx/press_on_feeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1l2xcyi</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>I am still learning</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2xcyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1l2vxut</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>My Kendrick Lamar GNX album inspired mani I wore to his SF show on 5/29 (swipe for the mock up I made for my nail tech)</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2vxut</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1l2w7ly</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Trans Pride nails</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vz67desl4u4f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1l2vms7</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>I need help with a badly damaged nail plate</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s8txljgvyt4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1l2uv1t</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>What polish do you think would be closest to this? I can't tell if it's a nude or clear glitter, but I'm obsessed with the super shimmery look. Credit: illuming_nail on IG</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b80s1367qt4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1l2ufsa</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Obsessed with this dusty blue-gray</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9af2l4zknt4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1l2uf3r</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Can you tell which is my dominant hand?</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2uf3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1l2uece</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>A cute lil Pride mani</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y5to56o7nt4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1l2u4ko</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Longest nails I’ve had</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9dc98joqkt4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1l2tt17</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>My GFs first attempt at nails.</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jefqpjvht4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1l2tpsl</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>First time at this salon - is this a red flag?</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2tpsl</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1l2td27</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>I have some damage on my nails, is this too much to have gel-x tips on?</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2td27</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1l2tscf</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>First time getting a nail art done. My nail lady did an amazing job!</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9zc0r9ipht4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1l2torg</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Does anyone know why this might be happening to my nails?</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8yyuxwsgt4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1l2to6q</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>butterfly nails!</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/puuz2mqngt4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1l2tmza</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>My nail artist slayed with these butterflies!</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2tmza</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1l2tlvh</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Happy Pride Month!</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2tlvh</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1l2tjr2</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Simple 🧿</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uqxqru4kft4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1l2teqb</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Highly recommend making your nails match your wedding color palette</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fj0tq1faet4f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1l2t71q</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>are these cute?</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nmu877bfct4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1l2t36g</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Spring/Summer Nails + Advice on Longevity</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2t36g</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1l2t4tg</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Happy pride 🌈</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sk7uxysvbt4f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1l2rkie</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Nail tech ripped my builder gel off and took my real nail with it</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l2rkie/nail_tech_ripped_my_builder_gel_off_and_took_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1l2sxjn</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Full Scream Ahead</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2sxjn</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1l2sq2t</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Fresh Claws</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1wrnxrd88t4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1l2skrd</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>stained glass nails</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s45f3ulx6t4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1l2sczj</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Feeling blue 🦋💙🐳🦕</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gk2d4lsy4t4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1l2scz7</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>So Cute</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xvm0typy4t4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1l2ry6z</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Pretty or nah??</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxz8ofh91t4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1l2rp8p</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Advice needed!!</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2rp8p</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1l2rgdo</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>All Natural</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2rgdo</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1l2qrta</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Protection for soft nails</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l2qrta/protection_for_soft_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1l2otl6</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>PSA for DIY nail girlies. Did you know your bonder may also have HEMA?</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2otl6</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1l2pfbe</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Supernatural nail experience?</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l2pfbe/supernatural_nail_experience/</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1l2q3uq</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Nail update</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k4gxuw8tls4f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1l2q27l</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Neon Pink!</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b38jdnmfls4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1l2ozma</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Gel fill?</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h96johr1ds4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1l2op6j</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>June Manicure 🧡🍊</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2op6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1l2nf12</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Are there press ons for curved nails??</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2nf12</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1l2nzj8</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>My nails by me ✨</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/copjqjbo5s4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1l2nppa</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>i usually dont like red on myself but i had a dream about this</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3myrd6p3s4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1l2njxn</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Dip powder girlies</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l2njxn/dip_powder_girlies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1l2n25f</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Did someone say we’re matching our nails to stuff?</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2n25f</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1l26q88</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>help! please! thyroid nails</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l26q88/help_please_thyroid_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1l2mjq0</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>My prom/graduation nails</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4vkoxs8nvr4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1l2lcaq</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>SINNERS nails - since today is the streaming release dayyy, apart from the ‘S’ everything is handpainted (Sammi’s broken guitar 🥹) - done by me</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2lcaq</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1l2l4fy</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Cat eye 🩷🤍</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2l4fy</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1l2ks0d</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Can I have classic fake nails with UV nail glue?</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l2ks0d/can_i_have_classic_fake_nails_with_uv_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1l2jn66</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>What I asked for vs What I got</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2jn66</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1l2ki2w</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Blue dragon set</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2ki2w</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1l2kf96</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>I'm so in love with these, but wearing them might be a nightmare</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2kf96</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1l2kelk</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>First attempt at press ons. How did I do?</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vmtgvvhrgr4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1l2kagd</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Recently started doing my own nails (past 6 months)</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2kagd</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1l2jdzq</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>I can’t get a fill for my Luminary mani for another 10 days unless they have a cancellation…they are a bit grown out lol</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r50y3nwf8r4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1l2j7ji</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Did my own nails for the first time?</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2j7ji</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1l2j55l</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>What would you pay for this?</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2j55l</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1l2iu36</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>june nails 🐞</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2iu36</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1l2isj0</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>New to doing nails at home - advice appreciated!</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/odk6jfzi4r4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1l2irq7</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Regular top coat?</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l2irq7/regular_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1l2ik7x</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Cloudy gel top coat</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2ik7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1l2idji</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Flowers</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2idji</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1l2i97s</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>How do you remove your Chillhouse press ons?</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ozbq050m0r4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1l2i6co</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>I hate my nails and have no clue what to do about it</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2i6co</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1l2i616</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>How can I improve my nails?</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2rrw0k7c0r4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1l2hmqg</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>almond or square for this darling twee inspired set ?</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2hmqg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1l2i0e3</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Lesbian nails for pride month 🧡🤍🩷</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2i0e3</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1l2hsn1</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>my new obsession: this baby pink shade 💕</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ew088fsxq4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1l2guw4</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>broken nail</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/794d738erq4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1l2hexl</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Never had my nails done before, are they good?</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2hexl</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1l2gp47</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Do you prefer liquid gel or gel x?</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l2gp47/do_you_prefer_liquid_gel_or_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1l2gmkz</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Any recommendations for products to fix peeling free edge?</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2gmkz</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1l2glj3</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Since we’re matching our nails to items…</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fdkj1hmkpq4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1l2g25b</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Spent 5 hours on this</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gth604xslq4f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1l2fzae</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Got my nails done!</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2fzae</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1l2fpfo</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Gel on bare nails vs fake</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l2fpfo/gel_on_bare_nails_vs_fake/</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1l2fijs</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Stained glass nails in Chicago</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/60zk9r01iq4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1l2fc6b</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Regular Gel or Builder?</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lkvrndwrgq4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1l2f4pe</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Do you like this shape or does this look off?</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7q7kjy7bfq4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1l2eyht</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Day 1 trying to grow out my natural nails using builder gel!</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2eyht</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1l2ey3x</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Felt a bit froggy</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2ey3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1l2ejt5</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Almost fainting at nail salon</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6ufb0i9bq4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1l27nln</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>What would you do with these nails?</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cm542c69no4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1l2d9v3</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Help!!!</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgw68mp42q4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1l2cq4y</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>new nails!!</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/js7ohou3yp4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1l2bjdf</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Gel allergy</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l2bjdf/gel_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1l26f1r</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Super glue and nails</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l26f1r/super_glue_and_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1l26fxb</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Allergy to Semi-Cured Gel Nail Strips (Ohora)  and Looking for Alternatives.</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l26fxb/allergy_to_semicured_gel_nail_strips_ohora_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1l28lsu</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Are these bad or am I just being paranoid?</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l28lsu</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1l2dxyg</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>I love a good chrome set!</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2dxyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1l2d8lw</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>One of my favorite jobs this month 🥰</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/239ceagv1q4f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1l2d847</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Barbie bling 💅</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kt1q6czr1q4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1l2d0r5</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Obsessed with magnetic polish!🤩</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jj0qd2na0q4f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1l2cx6o</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>cute blue nails</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2cx6o</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1l2bchl</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>blue nails</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2bchl</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1l2b8oz</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Masculine Nail Art Help</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l2b8oz/masculine_nail_art_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1l2axjr</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Bangkok Love</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/enkzvah4kp4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1l2ats4</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Same vibes or not?</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2ats4</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1l2a2ra</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>I enjoyed a lot getting my nails done until they've got weak and I took a break</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2a2ra</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1l2a2r4</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Happy Pride featuring KISS’s new impress summer nails 💜</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebhko5pkcp4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1l2zogc</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>My desk is messy af but at least my mani is satisfying</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wy2n5amm7v4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1l2zep0</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Similar shade reco</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/MM1EKMV</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1l2xgj6</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>can’t stop staring at my bug nails</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/30zmf2jnhu4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1l2x5lf</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Aquatic Skittle</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2x5lf</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1l2x18y</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Freehand abstract pride mani 🩷💜💙</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b97l4uygbu4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1l2wiv3</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Just proud of how I grew my nails, then how I shaped and polished them for the first time…all within two months!</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ltqda4cu7u4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1l2wh0t</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Book swatches</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nemrvyob7u4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1l2wanx</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Orly Pride Month</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h2sxlmqp4u4f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1l2vdna</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Autumnal vibes 🧡🩶</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2vd6o</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1l2v4ou</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Mooncat PFAHM vs BCB BTSLMY</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l2v4ou/mooncat_pfahm_vs_bcb_btslmy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1l2ty6y</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>can’t stop looking at my mani 😍</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2ty6y</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1l2u9vl</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>First time ordering from SheModern!</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cob2fbv2mt4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1l2te2z</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>CANADIANS!</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2te2z</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1l2tred</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Black shimmer polish?</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l2tred/black_shimmer_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1l2tlzz</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>EEEEEEEE!!!</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9cdvc74gt4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1l2thpp</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>All the colors were used 🌈</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2thpp</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1l2tdsd</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Any opinion on "Beter elite" glass files?</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l2tdsd/any_opinion_on_beter_elite_glass_files/</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1l2t7gd</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Does Lights Lacquer usually take a while to ship? Or is anyone else who’s recently ordered having a delay?</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l2t7gd/does_lights_lacquer_usually_take_a_while_to_ship/</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1l2t5nj</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Abstract stamp art</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2t5nj</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1l2n1wq</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>New to manis</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l2n1wq/new_to_manis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1l2seh6</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Yay gay! Squishy rainbow nails for Pride</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2seh6</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1l2sde0</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Psyche Minerals- The Ghastly Meltdown (April 2025 PPU)</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2sde0</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1l2rzvw</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Even in the dark we come through ❤️🧡💛💚🩵</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2rzvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1l2rzsw</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Finally bought sweet pea 🌸</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r52t645o1t4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1l2rj8l</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Not the gumdrop buttons!</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2rj8l</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1l2qazz</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>love this color</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2qazz</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1l2q3ww</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Discord drama summary</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2q3ww</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1l2q0ld</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Tips for filing down press on nails?</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hju2c9c3ls4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1l2psj2</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>You know it’s good when your husband comments on it</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pf6x65kajs4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1l2poha</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>The many faces of BKL spicy</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2poha</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1l2pig4</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Help me decide which polish I’ll wear next</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2pig4</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1l2p9h8</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Whose job was it to tell me that indie dip powders exist?? And Canadian too?? 🇨🇦</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2p9h8</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1l2oyuc</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Help find this color!!</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1mlzqtvcs4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1l2oiuh</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>🦋 Butterfly nails 🦋</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2oiuh</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1l2o8wv</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Are there press on’s for people who have a natural apex??</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2o8wv</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1l2o7hd</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>....is this too much?</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6sxnepyc7s4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1l2nnsn</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>My first ILNP order!!</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2nnsn</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1l2njv8</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Make staining work for you!</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3la1zfpn2s4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1l2mp55</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>how to use these nail art tools with regular polish?</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxd1utlmwr4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1l2mam0</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Having Nails When You Work With Your Hands</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l2mam0/having_nails_when_you_work_with_your_hands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1l2m2cv</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Recommendations for a pink polish similar to this color?</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qcu89k1asr4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1l2lznl</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Bee's Knees Lacquer - Toil &amp; Trouble</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2lznl</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1l2jajr</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>beginner May manis</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2jajr</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1l2lv8i</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Last week's mani</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2lv8i</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1l2ljwz</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Do you chop all or just one?</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l2ljwz/do_you_chop_all_or_just_one/</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1l2kozg</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Cirque Vice collection</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l2kozg/cirque_vice_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1l2knz7</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Ghosts of Hecate and Flower Child as Toppers</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2knz7</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1l2kbte</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>And to think this was the polish in the collection I was least excited about – Dragon Slay by Cracked</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2kbte</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1l2k5f4</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Pink Pony Club by Pahlish 🩷 My first mani of pride month!</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2k5f4</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1l2k0g7</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Please help me find this color?!</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2eodss27dr4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1l2jwcj</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Finally painted more than just my thumb nail.</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6lt43507cr4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1l2jaho</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>💚💙 ILNP Blue Lagoon 💙💚</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2jaho</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1l2ixwq</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Reminder to play with your toppers</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2ixwq</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1l2i6n3</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Nail ideas</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l2i6n3/nail_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1l2i0am</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Goodbye from Me</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l2i0am/goodbye_from_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1l2hc02</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>nude chrome 🫧</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rixmb8mmuq4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1l2hb7g</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Pride nails! Because just chrome ombre was too basic💅</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2hb7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1l2gpkc</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Big Apple Red 🍎</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2gpkc</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1l2gipr</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Abstract pride nail art 🌈</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2gipr</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1l2g42y</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>May Manis the 375th or so.</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2g42y</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1l2fy0h</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Paisley AKA Monkey</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2fy0h</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1l2fm6s</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>BKL “No One Believes You’re Dating”</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2fm6s</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1l2fk7d</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>I know Mooncat is kind of in the doghouse now, but…</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2fk7d</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1l2eunl</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Pride Manicure 1/???</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmgvty4ddq4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1l2es9y</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>I love all the what I wore in May posts! Mine, a bit late.</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2es9y</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1l2eqjd</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>This kicked off my massive nail polish decluttering spree</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h3ra0lskcq4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1l2ejdv</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Subtle pride nails 💜💙🩷</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o25s6yb6bq4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1l2dxfe</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Stellar Evolution</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k0uegf9x5q4f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1l2dtf8</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>nails and hair matching 🖤❤️</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gk4fdi726q4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1l2do2b</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Recs for ridge filler for horizontal ridges/lump. (Prefer a thinner, quick drying)</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l2do2b/recs_for_ridge_filler_for_horizontal_ridgeslump/</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1l2dhei</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Birthday Mani!</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2dhei</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1l2cqbg</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Latest manicures 🩵</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2cqbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1l2broq</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Favorite reds, pinks, peaches or berries- Indie Edition.</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l2broq/favorite_reds_pinks_peaches_or_berries_indie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1l2bdr5</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Tips for LESS topper coverage?</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2bdr5</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1l2aeqk</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Trying to recreate 1990’s Theon’s Ref</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujrvnxhmfp4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1l2a1tj</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>🌅Sunset Gradient🌅</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2a1tj</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1l29j7q</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>LOVING this one!! 😍</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l29j7q</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1l28mdg</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Anyone else wearing their pride flag as a mani?</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/524c5tb5yo4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1l289c5</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>First time! How do I get my cuticles/fingers neater?</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l289c5</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1l2yk1v</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Koi Fish Sticker Nails!</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2yk1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1l2y0xa</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>*repost* I am a licensed nail tech and I did these strawberries and daisies on a friend🍓🤍</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0p124su5ou4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1l2xw5d</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Super simple pride nails ( beginner attempt )</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p20hkeolmu4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1l2xrmy</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Can I put normal nail polish on gel nails? And take it off without ruining the bottom?</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1l2xrmy/can_i_put_normal_nail_polish_on_gel_nails_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1l2wv7w</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Watermelon nails for Summer</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2wv7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1l2w4j6</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Cat eye/glass nails 1st attempt</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/34agav7s3u4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1l2p2hh</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>First time sculpting and super happy with the result 🌺 my</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2p2hh</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1l2md3w</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>3D gel/clay recommendations</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1l2md3w/3d_gelclay_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1l2lpoz</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Tye dye(?) nails i did on my natural nails</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2lpoz</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1l2ju08</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Blue dragon set</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2ju08</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1l2iv49</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Made some new nails 😆</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bev5utvy4r4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1l2hmdg</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>almond or square for this darling twee inspired set ?</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2hmdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1l2h7ur</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Love Neon 🌈</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2h7ur</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1l2enc8</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Second time doing nails on my friend</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2enc8</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1l2cdcf</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Doodling bugs for my little sister</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d9z5n2qjvp4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1l28wp5</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Got these for my vacation to Hawaii last year and they came out perfect! Slayed as always by @sueznails</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f4aj8gjc1p4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1l28twc</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Fun and funky. Reminds me of saved by the bell! By @sueznails</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kha2033i0p4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1l27u4u</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>🌈🌈</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjhw06vgpo4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jun  5 08:13:00 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_08.xlsx
+++ b/data/collected_data/2025_06_08.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C721"/>
+  <dimension ref="A1:C931"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12690,6 +12690,3576 @@
         </is>
       </c>
     </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1l3tdti</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Which to wear to a purple and gold themed wedding?</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7q65v1fmc25f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1l3t7kp</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Just classic</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0pi4jpfha25f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1l3sny4</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>wine red nails!</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3sny4</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1l3s5jv</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>love looking back at my nail art journey and seeing how much I've improved in the past 5 years 🩷💛</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3s5jv</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1l3qxb0</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>BEST NAIL COMBO!</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cap1hfgak15f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1l3rv5v</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>flower frenchies… yay or nay?</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vuqxabguu15f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1l3qgo3</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Here fishy fishy set on my cousin!</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3qgo3</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1l3q70s</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Pedicure question</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l3q70s/pedicure_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1l3pzow</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Pompompurin Nails</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tq79m3cha15f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1l3pgzi</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Help with wedding nails</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3pgzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1l3pcje</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Onycholysis on just middle toes?</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l3pcje/onycholysis_on_just_middle_toes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1l3p4oj</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Is this wrong for my skin tone?</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/34j7lbny115f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1l3ou2i</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Builder gel help!</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l3ou2i/builder_gel_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1l3ou1o</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Cute spring themed nails</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3ou1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1l3ocww</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>is it bad etiquette to bring your own polish to an appointment?</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l3ocww/is_it_bad_etiquette_to_bring_your_own_polish_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1l3nxtt</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Today they asked me for this... Love the result 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bbd22ippq05f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1l3mmty</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>What are nail tips actually made of?</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l3mmty/what_are_nail_tips_actually_made_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1l3nmil</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Nail techs: what’s the best gift you’ve gotten or would love to get?</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l3nmil/nail_techs_whats_the_best_gift_youve_gotten_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1l3n37i</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Made my 2nd ever set of press ons🌈✨️</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3n37i</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1l3mf0f</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Weather map / infrared camera inspired nails?</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3mf0f</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1l3mjc0</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Love this design. GelX</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e46oagiae05f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1l3mbvm</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Color pencil/doodle nails</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6cc62k8gc05f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1l3m76t</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Builder gel nails</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mq3yd8jbb05f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1l3leh1</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>lil somethin for pride 🌈</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3leh1</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1l3lhas</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Bioluminescence Ocean Nails!</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3lhas</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1l3lfsc</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Recents on my bf and cousin 💜🐟</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3lfsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1l3lcz6</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Neon green aura 💚</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3lcz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1l3l490</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>I’ve been practicing</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aifwz75v105f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1l3l0ra</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>gold metallic nails have my heart✨</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uf129up2105f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1l3kmeb</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>What do I ask for (inspo: monika__nails on insta)</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qc3m9ndnxz4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1l3kp7n</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Soft gel brands?</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l3kp7n/soft_gel_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1l3k5o0</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>How do you make gel nails less chunky?</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jeg11ukrtz4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1l3k4d8</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>first time painting artwork :)</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3k4d8</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1l3k0ge</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>What can I do to lessen the pain during use of drill?</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l3k0ge/what_can_i_do_to_lessen_the_pain_during_use_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1l3k7ew</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>I just love these press ons!</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqelm5y5uz4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1l3k5z9</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Summer fun</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4car50yttz4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1l3k5w5</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>I hate when a picture doesn’t do a set justice</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/znefovoptz4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1l3jjch</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Back to my natural nails for the first time in a year 🫶🏻 I think I kinda like them and no biting so far 🥰🥰</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3jjch</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1l3jb5w</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Funky nail set 💅🏼</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9wfx0xu0nz4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1l3jahf</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>new color</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6p9lucsomz4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1l3j71s</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Mooncat - Dark Omens</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3j71s</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1l3iyrr</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>My boyfriend and I got a matching design 🥹</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m0o80atekz4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1l3inh3</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>finals are in two days, but i’ve just spent 6 hours cooking this</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3inh3</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1l3hykt</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Are pressons allowed here?</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hg1d0h6ucz4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1l3hjmb</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Birthday Nails! Astrology themed!</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d719ythr9z4f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1l3hhnz</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>started doing my own nails</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7wj6fq99z4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1l3hgh5</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Is there anything I can do about extremely short nail beds?</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l3hgh5/is_there_anything_i_can_do_about_extremely_short/</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1l3he4w</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Brittle nails that I tend to beat up inside gardening gloves several times a week. What can I do to grow them just a bit more?</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4u1afho8z4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1l3h9ki</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>ILNP Flower Child</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3h9ki</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1l3h9ja</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>I asked for clear chrome but got this pearly result. What went wrong? Concerned about clashing with my wedding dress 😣</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3h9ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1l3gf3i</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>I made a Shibari Set, but not by painting, by actually tying the nails with thread on a minature scale and then encasing them in Top Coat. How do you think it turned out? (:</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3gf3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1l3g7gw</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Happy Pride Month, Y’all 🌈</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jjwo9cc30z4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1l3g6x3</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Blue Ombre set</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3g6x3</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1l3fx2e</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>I let my nails grow out for the first time, any recommendations on what to do with them?</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hthhw6t1yy4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1l3fvcn</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Blue Cat eye</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/knmo1oqpxy4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1l3fuo9</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Should I still be using cuticle oil even though I have oily nails and skin?</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l3fuo9/should_i_still_be_using_cuticle_oil_even_though_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1l3frif</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Uhh a little help lol</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l3frif/uhh_a_little_help_lol/</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1l3f8k6</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>False info about chromes</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l3f8k6/false_info_about_chromes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1l3fnnw</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Love my toes. How did they come out?</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/knyo41u5wy4f1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1l3faok</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>whats the best type of nail adhesive? [brush on, nail stickers, liquid, gel] and why?</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l3faok/whats_the_best_type_of_nail_adhesive_brush_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1l3eusx</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Orchid nails</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3eusx</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1l3ekop</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>What happened to my nail?</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aur504sioy4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1l3em4y</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Favorite nail glue for press-ons?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l3em4y/favorite_nail_glue_for_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1l3e8vq</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>I love a RED set!</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y1l0nep9my4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1l3dvoc</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>New nails 🤍</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2xokc0vojy4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1l3dlpu</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>I had acrylics for the 1st time and I need to know if I should complain or if I am being too critical</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3dlpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1l3dg21</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Too much sparkle?</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzzum74ogy4f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1l3cm0q</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>My jacaranda blossom nails</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3cm0q</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1l3ci9j</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>I F up for the first time and I don’t know how to cope (inspo cocha_nail)</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3ci9j</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1l3ccxx</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>gel x popped off after less than 24 hours, is this normal for gel x?</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l3ccxx/gel_x_popped_off_after_less_than_24_hours_is_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1l3c8tf</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Nails of the day</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3c8tf</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1l3bu8e</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Why does this happen?</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p5q4s78f5y4f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1l3bm6g</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Tipping for nails?</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l3bm6g/tipping_for_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1l3blr4</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Question: how many times a day can I apply oil to my nails?</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l3blr4/question_how_many_times_a_day_can_i_apply_oil_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1l3bgck</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Green stilettos 💚✨</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oyc9dret2y4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1l3aud9</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>What is this on my nail</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3e984ldnyx4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1l3aozb</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>My new manicure 💅 these are my real nails with gel x ✨</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3aozb</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1l3ano4</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Calling All Nail Techs! Again lol</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9cxm6kjdxx4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1l3albb</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Chillhouse Soho?</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l3albb/chillhouse_soho/</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1l3ah8e</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Simplicity looks good on me..</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23qjz6b4wx4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1l3a4ib</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Press-ons (Glamnetics)</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3a4ib</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1l39ea4</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>I'm in love with my new nails 🌿</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l39ea4</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1l396h3</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>I like how they turned out</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iqy42yq3nx4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1l37dyv</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>What nail shape suits me best?</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l37dyv</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1l313w4</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>What is this on my nail??</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l313w4</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1l36lh9</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>what do you think?</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l36lh9</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1l3683e</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Four months of nail growth March-June (swipe for before)</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3683e</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1l38hm3</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Simple.</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l38hm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1l380l7</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Got nail art for the first time!</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7v1kvybxex4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1l37hwd</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>New set 💦</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tj3jmtwdbx4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1l37el8</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Working on the bling 💍</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l37el8</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1l36hli</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Pretty or not? What do you think?</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l36hli</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1l36e6x</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Matching. 🙂‍↕️🙂‍↔️</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rrxg5hk63x4f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1l369ik</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Love adding chrome for some fun!!</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h6dc9yn92x4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1l35wte</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Found a new nail tech who loves the art of design</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l35wte</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1l35n1a</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Customized a nailbliss press on set “rainbow run”.</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l35n1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1l35gkp</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Fresh Set 💜🧞🪁</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l35gkp</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1l35a6w</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Pretty happy with the length I’ve gained</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l35a6w</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1l3574q</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>done by me :)</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4197nvivtw4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1l34v9o</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>🍒</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/snbvydh8rw4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1l3s2vi</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Cracked Must-Haves?</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/guiehzp7x15f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1l3rkly</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Bee’s Knees on PPU</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l3rkly/bees_knees_on_ppu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1l3rj49</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Swatch sticks or books?</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4hh2msu3r15f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1l3r48g</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>MY GO TO ROUTINE!</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwew9s6fm15f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1l3qon4</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Essie - Mademoiselle</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7q1926sh15f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1l3qb62</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>On a mission to find what colors I like under Foxfire</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3qb62</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1l3q93h</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Custom-made Metal Nails</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://snailworks.store/products/custom-made-solid-metal-nails?variant=55567521022326</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1l3q3be</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>My first Pride mani of the month!</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3q3be</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1l3pxqg</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Shipping Heads Up</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l3pxqg/shipping_heads_up/</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1l3p6j7</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>ISO a true burgundy polish</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l3p6j7/iso_a_true_burgundy_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1l3ot9n</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Are you floral?</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r0rlz5fvy05f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1l3nl0d</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Racing stripes 🚙</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jauycadin05f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1l3oiro</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Dupes of At Last Lights Lacquer</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gokmrwh3w05f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1l3ohe2</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Drown My Demons</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xt3whklcv05f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1l3nxn7</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>💅✨️💜</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9jne1doq05f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1l3nuhw</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>La Petite Mort needed some nudis</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3nuhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1l3n8id</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Ignore the mess!</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwlkqguhk05f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1l3m8al</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>do yall prefer pictures or chatty videos?</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j4q4ud0ib05f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1l3ly3u</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Hubba bubba</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rfb10m13905f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1l3lu7y</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Can we pls appreciate this beauty even with my terrible nail lengths and shapes..🫣</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3lu7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1l3lo9i</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>does nail polish really boil down to body chemistry?</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l3lo9i/does_nail_polish_really_boil_down_to_body/</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1l3l4el</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Dudley Nudshite</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sur4818w105f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1l3krn4</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Cosmic Polish's Sub-Zero gives me LIFE</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3krn4</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1l3keaq</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Dupe request please! Mooncat The Dark Side (discontinued) or LA Colors Glitter Vibes Time To Shine (doesn't ship to Canada). Been searching for the perfect black glitter polish, chunky glitters preferred. Thank you for any suggestions!</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3keaq</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1l3k8nu</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>These look crazy in setting sun!</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/opil6qaguz4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1l3k36y</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>My favorite set I’ve ever gotten 🥹🍒</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3k36y</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1l3k079</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Birthday skittle 🥳🐛🪲🐞</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3k079</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1l3jwiy</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>ILNP Misfit - Happy Pride!!</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3jwiy</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1l3jnrf</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>How long does it take for Polished for Days polish to dry?</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l3jnrf/how_long_does_it_take_for_polished_for_days/</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1l3j7s4</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>PSA: Canada to US Shipping/Tariffs - Recent experience</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3j7s4</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1l3j3y5</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>What's happening?</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3j3y5</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1l3ipid</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Doom Loop!</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3ipid</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1l3img5</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Making Apocalypse Jokes Like There’s No Tomorrow</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3img5</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1l3ibgr</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>So how are we going to be recreating Elphaba's nails?</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mtdcirqbz4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1l3i62k</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Happy Pride 🩷💜💙</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3i62k</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1l3hur6</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>swatches of the Bkind polishes I have</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3hur6</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1l3hu7g</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Looking for a new indie brand for a summer haul</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l3hu7g/looking_for_a_new_indie_brand_for_a_summer_haul/</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1l3ekyi</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Can you re-apply a pop off set like press ons?</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l3ekyi/can_you_reapply_a_pop_off_set_like_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1l3hkqq</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Flower Power 🌸💜🌸</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e6sviouz9z4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1l3h7xp</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Weird line? And nail advice?</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3h7xp</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1l3h6o1</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Pride mani on me and my 12yo</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3h6o1</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1l3gsnt</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Cracked Arcana Collab polishes arrived 😍</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3gsnt</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1l3gmyu</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Behind again by Emily de Molly 💚🍃</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3gmyu</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1l3fwye</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Oil slick nails</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/dE75zaK.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1l3f6nv</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>I was going for rainbow but missing a few colors. Love it anyway</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3f6nv</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1l3f1fu</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Babysitting a Laquerista in the Making!</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3f1fu</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1l3eqwk</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Been doing my gel nails at home for a few years. Anywhere I can improve?</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3eqwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1l3ehcr</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Iridescent seashell nails from my beach elopement 🥰</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9332s82wny4f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1l3eg1x</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Obsessed with my little collection</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/37ioc3bnny4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1l3e9on</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Curved Nails</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l81555ffmy4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1l3amlx</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Nail stands/trays for press ons ❤️</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l3amlx/nail_standstrays_for_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1l3dzqm</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Am i tweaking</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3dzqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1l3dstt</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>HEMA in standard polish?</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l3dstt/hema_in_standard_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1l3ck15</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Opinion on Olive Ave?</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l3ck15/opinion_on_olive_ave/</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1l3civr</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>ILNP Revival OMFG</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3civr</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1l3cd9v</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Having fun with my dotting tool!</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3cd9v</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1l3c02s</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>My nail and I are in splitsville - help!</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l3c02s/my_nail_and_i_are_in_splitsville_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1l3brrb</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Beginner mani - first Cirque order!</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3brrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1l3bhus</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>My first try with pigment flakes</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3bhus</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1l3bebd</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>🌙😻 holos and glitters</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3bebd</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1l3b2kb</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>More Pride Nails! 🩷💛🩵</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3b2kb</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1l3atw3</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Info about these cute little sloth polishes? 🦥</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3atw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1l3aldr</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Polishes similar to the Dust to Dust collection by Death Valley Nails?</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l3aldr/polishes_similar_to_the_dust_to_dust_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1l39zst</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>holo top coat recs?</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l39zst/holo_top_coat_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1l39ufo</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Birthday Rewards</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l39ufo/birthday_rewards/</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1l39raa</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>🇮🇹 Italy nails 🇮🇹</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l39raa</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1l39hb9</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Mooncat Blood Moon vs Holo Taco Dead Petals</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l39hb9/mooncat_blood_moon_vs_holo_taco_dead_petals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1l39b7o</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>some simple ✨pride✨ nails</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l39b7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1l3986a</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>I'm obsessed with this color 🦢</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sh0ffmrfnx4f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1l3966e</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>They look really bumpy in pictures but I still wanted to post them (they don't look as bad in real life)</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yi0b3h91nx4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1l38yny</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>My favorite press ons I’ve done yet</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l38yny</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1l387kq</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Top coat recommendations for Solars</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jge54beagx4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1l385fp</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>EO Essie coverage</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l385fp</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1l36zhr</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>How did you learn to file your nails into desired shape?</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l36zhr/how_did_you_learn_to_file_your_nails_into_desired/</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1l36q11</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>twi_star (Angel) Disturbing Instagram and YT update?</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l36q11</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1l364f1</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>🐸Kermit the Frog🐸</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l364f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1l360oj</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Pride mani: week one</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vmk5ta6e0x4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1l35wlc</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Happy Pride Month 🖤💜🤍💛</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l35wlc</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1l35tr9</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>“You have too many ILNPs you haven’t worn” skittle!</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iqd1b2dyyw4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1l35pgn</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>not sure if this is cute or not but it’s summery</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l35pgn</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1l35be2</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>🧚‍♀️ she was a fairy yuh yuh… and these are her nails✨💅🏻</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l35be2</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1l3564k</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Sally Hansen primer</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l3564k/sally_hansen_primer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1l34w3f</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Wedding nails!</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8rxrscdfrw4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1l34gtz</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Play ball! ⚾️🏟️</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l34gtz</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1l345zt</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Love me some Lurid</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l345zt</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1l33n07</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>MC Sagebrush 🌿</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l33n07</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1l32hjg</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>ILNP Thundercloud</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l32hjg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1l324ue</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Nailed it</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ei7o5up61w4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1l321mp</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>OG pride flag!</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l321mp</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1l317fv</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Okay but really, do you also get overstimulated by your long nails?😭</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l317fv</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1l30dxk</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>He proposed – and I was wearing my favorite polish!</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l30dxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1l3qnnx</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Deep red cat eye with gold color shift?</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1l3qnnx/deep_red_cat_eye_with_gold_color_shift/</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1l3pgbd</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>what kind of technique and polishes would give this sort of barely ombré effect ?</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r2t4ol21515f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1l3pfcd</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Just finished this set on myself! 🧡🌞🌼💖</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3pfcd</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1l3o4e8</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Cat Eye Glue</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1l3o4e8/cat_eye_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1l3n2xu</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>🛸alien / space press-ons👽 ࣪ ˖͙͘͡★</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3n2xu</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1l3kphq</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Happy pride!!</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3kphq</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1l3i8ma</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Fresh claws</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0vlfzbswez4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1l3gk02</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>I made a Shibari Set, but not by painting, by actually tying the nails with thread on a minature scale and then encasing them in Top Coat. What do you think? (:</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3gk02</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1l3gfmu</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>tips?</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3gfmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1l3fvi2</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>June nails!</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3fvi2</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1l3f7ie</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Happy pride!!!</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3f7ie</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1l3eqqx</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Can I re-apply a Pop off nail set as press ons?</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1l3eqqx/can_i_reapply_a_pop_off_nail_set_as_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1l3cvdm</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Press-on i made〜</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3cvdm</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1l3b5ua</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>i need some advice !</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1l3b5ua/i_need_some_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1l3ai0a</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>It's nothing as good as everyone else's, but I was pretty happy with how my first attempt came out :)</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e2rpq0v9wx4f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1l38ohf</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Something colorful ✨</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yp5vf8wljx4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1l36a8j</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Acrylic overlay ready for two CC shows in London 🤠♥️🇺🇸</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dw7xnr6f2x4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1l33vas</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>My friend wanted some nails for her green drag queen costume, do you think I delivered?</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l33vas</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1l33s9y</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Zebra print stamping + gradient</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mzu5d96shw4f1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jun  6 08:12:44 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_08.xlsx
+++ b/data/collected_data/2025_06_08.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C931"/>
+  <dimension ref="A1:C1132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16260,6 +16260,3423 @@
         </is>
       </c>
     </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1l4mxzc</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Recommendation for a foolproof nail file?</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l4mxzc/recommendation_for_a_foolproof_nail_file/</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1l4m6v8</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>First time getting my nails done. Please be honest, are they bad? Not that i can change them but i kinda feel dishearted by the criticism i recieved for it. It's my graduation ceremony in a few days and I was told sth like crimson would've been more extravagent.</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oahi2s13a95f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1l4kps3</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Gel question</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l4kps3/gel_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1l4ljvn</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>pmo this is new i told her all the way close to proxima fold abd she said yeah but dayum :(. also its not grown out my nails don't grow fast</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4ljvn</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1l4ljbq</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Throwback to my favorite nails evaaa 🐜</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4ljbq</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1l4l9om</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>What’s a good/fun nail design to wear with a yellow dress?</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l4l9om/whats_a_goodfun_nail_design_to_wear_with_a_yellow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1l4ks8o</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Just spent $97 on a set I hate — how can I tone them down without starting over?</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t36v0r8mu85f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1l4kf3g</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>🍒</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4kf3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1l4k4sf</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4k4sf</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1l4j4w6</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Y2K vibes</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bgk09r7kd85f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1l4ix8j</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Toma-toes 🍅</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ygefq1aib85f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1l4fuia</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Nail emergency! Wedding in two weeks</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l4fuia/nail_emergency_wedding_in_two_weeks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1l4fqpl</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>I am crazy obsessed with these!!</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4fqpl</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1l4ijjb</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>My best friend's manicure for her graduation</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4ijjb</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1l4iizr</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Thought I’d try something different today!</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4iizr</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1l4ib0g</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>New set- Mani/Pedi ❤️💜</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4ib0g</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1l4hykl</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Plankton Nails</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/alfpjtjb285f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1l4hwk8</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Help: Acrylic nails popping off after 2 weeks on short nails?</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l4hwk8/help_acrylic_nails_popping_off_after_2_weeks_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1l4ho4z</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Fresh french tips</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4ho4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1l4hm79</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Berries and Moos Press ons</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4hm79</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1l4hdfr</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Redid my nails today! (still learning)</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4hdfr</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1l4galf</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Tips for at home French manicure?</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rme6ozlmm75f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1l4fohj</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Does anybody have nails that reminds you of this?</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vipzd3i3h75f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1l4fhps</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Gel-X at home</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l4fhps/gelx_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1l4f9p8</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>DND Overseas Diva ⚓️🏝️</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vfgxauz9d75f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1l4f4mv</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Cherries 🍒</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4f4mv</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1l4f2aw</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Summer Nails</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/no5vk2kdb75f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1l4d8wg</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Salon experience help</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l4d8wg/salon_experience_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1l4errw</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Obsessed with this light pink, so clean and pretty</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c7msxqos875f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1l4epl4</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>I'm still learning. I did good or naaah?</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/twwhw7s9875f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1l4ekqn</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Reflexive blue nails 🕺☄️</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4ekqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1l4ej8v</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Recommendations/help</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4ej8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1l4ehmm</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>First time French Tips on natural nails</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4ehmm</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1l4ehcl</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Help a long nail newbie</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l4ehcl/help_a_long_nail_newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1l4e9z5</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>I need some honesty. Are these too big for me? I can't tell if they're too wide or long or just right.</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4e9z5</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1l4e60z</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>First set of almond Summer fruits</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4ts2lig375f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1l4e0cq</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Nintendo nails🍄☁️⭐️</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h5udkdu2275f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1l4dtks</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>I don't know what I'm doing wrong.</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4dtks</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1l4dg8h</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Killed her husband 🐯 whacked him</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4dg8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1l4d3gj</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>stained glass inspired nails</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q2m5txybu65f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1l4d5zu</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>hers &amp; hers for our anniversary &lt;3</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eqz88prvu65f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1l4cnp2</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>❤️🧡💛Candied Pride💚💙💜</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8xojxqusq65f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1l4c9bz</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Fill or full new set?</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l4c9bz/fill_or_full_new_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1l4bzf4</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Nails for a wedding in Florida where my dresses are blue and orange 🍊💅🏽🧡💙</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1vrsi9adl65f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1l4b5em</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Fist time with blooming gel</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iy2x0ic8f65f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1l4ahro</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Hey friends! Do we know of any subs specifically for men who paint their nails?</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l4ahro/hey_friends_do_we_know_of_any_subs_specifically/</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1l49t4y</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Tip question</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l49t4y/tip_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1l49nor</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>So happy with these 🩷🌺👙🦩</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v89sae1f465f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1l49fq6</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>My pride nails 💅</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/srj1kgqt265f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1l4944b</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Pretty obsessed with my new set</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2jj94d3i065f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1l48y8q</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Square or Rounded/Almond?</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l48y8q</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1l48s84</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>My simple summer (Pre Pride) nails! I do them myself, so please be nice 😂🫠</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zls3xs23y55f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1l48elp</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Any way I can save this 🥲</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l17xejicv55f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1l4858t</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>are my nails mature yet?</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/umo9fnv7t55f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1l47zq3</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Nothing like getting a fresh set before going on holiday 🪩</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t9ft757es55f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1l47ihm</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>I'm a Man Growing My Nails Out</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l47ihm</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1l47eex</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Garden party vibes</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rmmlg31ao55f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1l46ual</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Acrylic Overlay w/ gel polish. Couldn’t be happier! 🤍</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r4z7tjlbk55f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1l46rov</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>We’re Leaving the Planet</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5gdfmmirj55f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1l45u6c</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>nail polish still listing no matter what I do</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l45u6c/nail_polish_still_listing_no_matter_what_i_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1l462ln</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>One of my favorite sets I've done</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l462ln</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1l45wgd</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>🖤🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n0socfhtd55f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1l45kqz</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Cute junk nails</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l45kqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1l45ei1</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Cat eye 🐱 black and border</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sh5wqusaa55f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1l45e9p</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Spring floral</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l45e9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1l4597b</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>are these bad?</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4597b</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1l44yf3</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>My non-dominant hand builder application is getting better!</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l44yf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1l44k0c</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>First Time Press Ons on short and small natural nails</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l44k0c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1l43ph7</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Few questions?</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l43ph7/few_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1l42ejv</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>My favourite salon is an 8hour flight away from me</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xbbiia3dp45f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1l431wl</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>My nails this month! Which picture is the best?</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l431wl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1l43l5l</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>This is the manicure I got today I think it looks good</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/236tr0vjx45f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1l43f2j</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Lifting of gel manicure help</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p3027duhw45f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1l43d32</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Loving the Phillies powder blue vibes</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/afe9myz2w45f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1l432or</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>beginner sets</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l432or</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1l42sdx</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Rainbow Holo</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vo542da0s45f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1l42otk</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>how damaged are my nails</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gt991gzfr45f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1l42oed</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Summertime nails 🍊🍉🪻</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kkl62kacr45f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1l42n0f</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>I've been busy with this set today.. Pretty, right?</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l42n0f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1l3uxm9</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>I just did these</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3uxm9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1l424ra</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Is my nail prep okay?</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sdku5jthn45f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1l424cs</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Holiday Nails 🍒🌸🐊</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/amzt3c0fn45f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1l3vpt5</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Can I have a bath with acrylic nails?</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l3vpt5/can_i_have_a_bath_with_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1l41p87</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Thought I'd treat myself on this rainy Thursday afternoon</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o6c8n372k45f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1l41g0z</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>birthday manicure ✨</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l41g0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1l40xb9</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>First time getting gel nails - good or not?</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l40xb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1l40qrz</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Bee's Knees Lacquer - I'm Not Afraid, Not of You</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v0j5m4dld45f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1l3y2j1</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>I love my natural nails. Nothing on them!!</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3y2j1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1l3ukkv</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>1st time w/ builder gel vs. 2nd time</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3ukkv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1l3ujjl</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>can u change ur design and is it okay to do it</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l3ujjl/can_u_change_ur_design_and_is_it_okay_to_do_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1l3u10h</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>One Mani At a Time</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3u10h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1l4mk35</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>acetone not cleaning nail brushes</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l4mk35/acetone_not_cleaning_nail_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1l4l8om</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Finessing the Holo Taco chunky glitters into a Pride rainbow!</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4l8om</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1l4k4gs</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Regular polish nail art inspo?</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l4k4gs/regular_polish_nail_art_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1l4js4p</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>need tips/recs on structure/builder gel for reinforcing natural nail + how do regular polish on top</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l4js4p/need_tipsrecs_on_structurebuilder_gel_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1l4jq6g</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>What to do when a formula sucks and thinner isn’t helping?</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l4jq6g/what_to_do_when_a_formula_sucks_and_thinner_isnt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1l4iv4v</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Can anyone recommend a similar color to lemming lacquer's Josh the lover of tomatoes</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5w39bs4y985f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1l4ijl3</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>ISO starry, starry night dupe?</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4ijl3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1l4igvp</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Bubbles in Petals for A Narcissist</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tkdxm1c2785f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1l4hxp5</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>help i keep having lobster hands</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d05ld592285f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1l4hs6n</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>ISO Fenty Diamond Bomb in a nail polish.</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l4hs6n/iso_fenty_diamond_bomb_in_a_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1l4grec</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Birthday</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/loybhco1r75f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1l4hkjy</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Back to simple nubs 🥲</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7xkreksky75f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1l4hdkr</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>salon perfect top coat discontinued??</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bwq8dyiqw75f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1l4h4fg</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Magnetics -- mesmerizing af -- grainy af, too 🧲💅</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ljhiqzw4o75f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1l4gqms</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Multi-Brand Polish Haul Video</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zt6bm5ysq75f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1l4gmwv</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Happy Happy Pride! 🥰🥳🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4gmwv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1l4g098</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>PPU, LBOH, Uno Mas, and BKL Haul</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4g098</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1l4fspi</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Reflective Rainbow for Pride Month</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n6f39hsig75f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1l4f8gw</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>ILNP - Shooting Star</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1slj5tuc75f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1l4f6f6</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Penelope Luz La Ville Lumiere a close dupe for PFD Goblins and Ghoulies??</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l4f6f6/penelope_luz_la_ville_lumiere_a_close_dupe_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1l4f4hc</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Give It Back Tenfold - Bee's Knees</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v777ym8wb75f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1l4eu1r</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Nails with Nugget: Pride Nails 2/??</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gm0r3inc975f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1l4egox</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Happy Pride Jelly Sandwiches!</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4egox</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1l4ef12</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Sally Hansen Diamond Strength</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4ef12</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1l4edyn</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Thoughts on textured pearl? Ugly or pretty?</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xtmbp0ze575f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1l4e94r</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>I fell while hiking and I think I broke a nail under my biab polish :(</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l4e94r/i_fell_while_hiking_and_i_think_i_broke_a_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1l4dtw3</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Is nail polish thinner worth using?</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l4dtw3/is_nail_polish_thinner_worth_using/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1l4dkpf</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>💖Barbie Nails 💖</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4dkpf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1l4djzf</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Blue and chunky glitter</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2co6ne23y65f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1l4din3</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Upside Down Bicycle Ice Cream🚲🍦🍧</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4din3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1l4dder</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>I love how this combo turned out</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4dder</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1l4cgwp</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>When does Cracked Polish ship orders out?</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l4cgwp/when_does_cracked_polish_ship_orders_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1l4c85p</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>The HT Cottagecore greens match my favorite keebs perfectly!</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4c85p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1l4biit</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Camping wedding nails</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4biit</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1l4b8de</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Obsessed with the sparkle ✨️</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4b8de</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1l49ao1</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>I Just Want to Spank it Out of Him 💚💜😜</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l49ao1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1l4abva</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Nails for the weekend.</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zebwud1c965f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1l4a7kb</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Nail Break :(</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yuhy2h7g865f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1l4a6l2</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Is this look possible with JUST regular polishes? If so, which polishes do you recommend?</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/00wdtss8865f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1l49vss</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>So prettyyyy</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2rrr6gxw565f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1l49uno</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Cirque - La Dolce Vita</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f86zlj2t565f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1l49t1t</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Was Holo Taco Matte Taco reformulated at some point?</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l49t1t/was_holo_taco_matte_taco_reformulated_at_some/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1l4886j</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Soapy, sparkly nails?</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l4886j/soapy_sparkly_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1l4815v</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>My vacation nails holding up through snorkeling/swimming!</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46ds2g6os55f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1l47v0s</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Dirty Ombré</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zrr5dsrfr55f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1l47ffw</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Garden party set</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qql0oh6ho55f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1l46v0o</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>We’re Leaving the Planet</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5gdfmmirj55f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1l46u67</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Cornea Killer</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l46u67</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1l46q8m</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Clionadh-Dreamscape</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l46q8m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1l46irz</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Regarding user who was banned for 7 days for what was perceived as undisclosed market research. Unban and apology</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l46irz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1l46irk</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>regret</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i03tdc41i55f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1l46gia</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Can I use a gel top coat on regular polish?</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l46gia/can_i_use_a_gel_top_coat_on_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1l465t4</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>I can create a lapis lazuli, right?</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6wkr50if55f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1l45ksf</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Three week update on healing my cuticles. Lifelong picker that has never painted my nails. Anything else I should do before I try?</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l45ksf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1l44vhs</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Indomitable is THE purple I've been searching for</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4ze2g3r655f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1l44t23</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Twinning with my energy drink!</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l44t23</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1l44nt4</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>A day of work: a story told by nails</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l44nt4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1l44e0o</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Achieving shelf-actualization</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l44e0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1l44cy5</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Decided to try and do my own nails with builder and gel, lots to learn but I had fun! Yes, that’s supposed to be a shell 🤣</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xtucxh78355f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1l44ah2</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>What is this tool and how I get one?</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/92ua75jq255f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1l43wlx</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>River Styx @ Lake Tahoe</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l43wlx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1l43ulb</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Gel lifting help</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y6konxgkz45f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1l43csl</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Summer Metallics</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l43csl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1l4392s</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>posing (and posting) is hard, but happy pride! 🏳️‍⚧️</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4392s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1l437ho</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>We’re back, bahía!</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0p6opshxu45f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1l42s5g</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Purple Party Monster</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l42s5g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1l42auj</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Which order should I do?</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l42auj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1l41rpw</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>skittles???</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l41rpw/skittles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1l41ebw</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Glitter is not my style but this is so pretty!</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l41ebw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1l40r1i</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Bee's Knees Lacquer - I'm Not Afraid, Not of You</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jl9z14end45f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1l40op4</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Cursed with bendy, fragile nails, any tips?</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l40op4/cursed_with_bendy_fragile_nails_any_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1l40ef4</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Neil Degrasse Tyson inspired nails with Mooncat Millennia 🌌</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l40ef4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1l3zshg</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Looking for the non-magnetic equivalent of ILNP's Amped</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l3zshg/looking_for_the_nonmagnetic_equivalent_of_ilnps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1l3zdlg</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Finally here to update</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3zdlg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1l3yfxf</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Oz green</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3yfxf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1l3yf6f</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Nail polish over acrylic nails</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l3yf6f/nail_polish_over_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1l3wsb2</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>First Time Matchy Matchy 😍</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8t3amwbg35f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1l3wnce</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Two colors: how do we use two?</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ouooxe6ye35f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1l3vq8u</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>My precious</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8zc8j018535f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1l4m38h</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>My first self nail tip extensions with cat eye gel</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4m38h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1l4kut1</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Jiraikei nails (not a pro)</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wbpse2nhv85f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1l4k4ke</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Ombre/gradient without latex?</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1l4k4ke/ombregradient_without_latex/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1l4h246</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Bright &amp; Bold - Multicolor French Tips! 💅🌈</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7nc5zrat75f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1l4gyvb</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>sick nails for a concert</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4gyvb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1l4fw7f</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Best summer nail ideas</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xpnvqnl1j75f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1l4frca</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>beginner!!</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4frca</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1l4e6tq</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>I do my own press ons. I think they’re cute 😃🌻💛</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4e6tq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1l4dz4x</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Billie Eilish inspired nails</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4dz4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1l4dvjf</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Look at my nails 😭😭</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3m67rhdx075f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1l4drdc</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Lavender Set 🧞💜🪁</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4drdc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1l4czg2</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>My nails today</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kpsu846ft65f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1l4cof5</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Summer vibe nails (beginner)</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4cof5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1l4ch71</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Soul eater nails</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vkw3adhcp65f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1l4c1cb</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Nails for a wedding in Florida where my dresses are blue and orange 🍊💅🏽🧡💙 by my magical nail artist fairy 🧚 @nails_emmywynn</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/729etxovl65f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1l4b6rs</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Saw this a while back done in black and white. I had to do it in pink.</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i58h365if65f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1l49jk3</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Labubu nails</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l49jk3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1l499qc</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>😋🖤</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s2fsaeim165f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1l49905</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>concert nails 💅</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/df141akh165f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1l47ve2</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Calling all artists!!</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vnkjt4fir55f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1l47lmf</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Pride Nails!</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ernwlewlp55f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1l47fx0</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Garden party set</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qmfwwdiko55f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1l47cbk</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>We’re Leaving the Planet</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bjcmtv1vn55f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1l475f2</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>First set</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1l475f2/first_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1l46t5e</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Lisa Frank Inspired Y2K Nails 💜🩷🖤</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l46t5e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1l461b5</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>My nails this month</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l461b5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1l45hbr</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Cute junk nails</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l45hbr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1l44bgf</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Tried doing my own nails with builder and nail gel, lots to learn but it was fun! (That’s supposed to be a shell 🤣)</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/benlp8hx255f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1l40eno</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>did my nails for the first time</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l40eno</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1l3ukz6</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>is it still OK to not use gel polish?</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/72isxecsr25f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1l3ucca</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Attempt at lighter nail design on myself</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9heoutso25f1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jun  7 08:10:50 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_08.xlsx
+++ b/data/collected_data/2025_06_08.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1132"/>
+  <dimension ref="A1:C1350"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19677,6 +19677,3712 @@
         </is>
       </c>
     </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1l5fnl0</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Nails for pride 🌈</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0j5lxsd9qg5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1l5erto</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>I am desperate. How do I take off this nail gem?</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5erto</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1l5eq9s</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>💙 (literal)</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pfyqhfqweg5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1l5ela1</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Gel Nails</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l5ela1/gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1l5eb32</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxea8a9w9g5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1l5e6qt</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Perfect little pressies my friend/tech made 🌼💛</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5e6qt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1l5e59v</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Feelin froggy? 🐸💕</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6u2ezoqy7g5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1l5dz9z</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>first summer set</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5dz9z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1l5dyv5</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Should a nail artist tell the price upfront?</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l5dyv5/should_a_nail_artist_tell_the_price_upfront/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1l5dkri</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>My first gel x set in a years</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9e3j66291g5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1l5dac7</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>I love my nail lady</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hznhwv2vxf5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1l5c274</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Wide nail bed.</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l5c274/wide_nail_bed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1l5c99k</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>First time using nails this long!</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y2cb0swpmf5f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1l5b33o</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>nail specialty needed</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/918ht1o89f5f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1l5b4ar</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Toni Collette’s Nails</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5b4ar</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1l5blme</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Turning 30 this week and went with a simple look 💅🏽</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5blme</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1l5bj7o</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Do I pay to have these redone again or am I being picky?</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5bj7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1l5bgii</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Hard gel on my natural nails!!</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5bgii</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1l5bayi</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Nude for hike💅✨</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7diqsk7tcf5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1l5b6n5</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Spring sky blue with flowers</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgdwzj5mbf5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1l5b2zt</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Adorable structured gel manicure I did on my best friend! 🤩</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/noif45ilaf5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1l5b2h8</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Pride Nails</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5b2h8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1l5affj</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Please help 🥲</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0bljj7o84f5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1l5ah8p</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Please tell me what nail shape I should have.</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5ah8p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1l5akav</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Blue flowery French</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x966tyyj5f5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1l5ah83</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>In love with the final result 🥰🫶🏻</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5glvnnvp4f5f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1l59k90</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Ski Slope/jump nails Do I need them removed?</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l59k90</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1l59g83</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Fruit nails- what do you think?</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l59g83</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1l59g7h</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>A $25 builder gel kit, half a YouTube tutorial, and 1.5 hours of my time and i gave myself a beautiful manicure</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l8c7hv8xue5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1l58yki</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Birthday set 💖🐚</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zx3rzgt7qe5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1l58trv</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>💚🦋</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l58trv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1l58kj1</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>hard vs soft gel for fixing curved nail?</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l58kj1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1l5804s</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Another Kali Uchis inspired set 🦋</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5804s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1l57re0</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Am I supposed to put cuticle oil on my acrylics? If so how often? Just the cuticle or the whole nail?</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l57re0/am_i_supposed_to_put_cuticle_oil_on_my_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1l57rcs</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Pearl</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l57rcs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1l56mnm</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time!!</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l56mnm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1l5733p</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>How bad are these</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5733p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1l57f5d</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>new nails!! what do we think?</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18xlahj4ce5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1l57elh</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>anybody know of Gel X nails for REALLY SMALL nail beds?</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l57elh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1l5727l</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Question about builder gel</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l5727l/question_about_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1l56xgv</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Glitterbel base issue</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l56xgv/glitterbel_base_issue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1l56vta</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Advice/opinions</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l56vta</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1l56fuk</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>How much should I charge?</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l56fuk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1l55ybi</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Pride Nails!</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ehwuckrtzd5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1l55sh2</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Give me some winter nails ideas peeps!</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l55sh2/give_me_some_winter_nails_ideas_peeps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1l54sm9</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Air bubbles after gluing on tips</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l54sm9/air_bubbles_after_gluing_on_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1l55aza</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>What products to use and in what order / Gel manicure</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l55aza/what_products_to_use_and_in_what_order_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1l55866</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Hi, I just got my nails done. Do you like that color?</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zclc6v4wtd5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1l557r5</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Rainbow nails</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pju9m5wstd5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1l54y85</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>galaxies at the gym</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a4w3zgaprd5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1l54kkj</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>What do you think of this shade of blue?</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ref011sod5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1l54hhc</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Powder Pink by DND</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ih5outu2od5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1l53dky</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Harley Quinn inspired!</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4qyjj6lfd5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1l53ftg</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>DIY tips for pride 🌈</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v433lum2gd5f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1l53bir</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>She has 3 looks</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l53bir</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1l53ai0</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Aquarius birthday nails</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l53ai0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1l5394x</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Watercolor floral!</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5394x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1l5372u</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Wicked vibes!</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5372u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1l5328j</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Reminds me of starburst!</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5328j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1l52pfb</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>First time doing gel nails. Tips?</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l52pfb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1l52skl</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Which hand looks better?</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l52skl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1l52ron</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Should I cut them?</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qaqi2bowad5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1l52fll</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>I think this blue should have been darker …</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxdfjtkd8d5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1l520u1</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Disco balls and clowns to celebrate pride month 🥳</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l520u1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1l51w8a</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Added a decal for pride. 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z2kmmwyd4d5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1l51mql</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Pride nails!</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l51mql</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1l51b21</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Happy Pride Month! I hope you like my bi-flag nails!</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sczwlvvtzc5f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1l50y47</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>My favorite set I’ve done so far.</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l50y47</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1l513v6</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Tried out a new nail tech and I’m unsure how I feel.</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rjif3ngdyc5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1l50zsu</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>French! 🤍</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cag6v9hjxc5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1l50wzf</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Pride nails!</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l50wzf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1l50tcb</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Obsessed is an understatement</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lwjr8rt6wc5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1l50nd9</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>I love my nail lady 😍🫐</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l50nd9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1l4z1ma</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>How do I prevent my gel polish from lifting?</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l4z1ma/how_do_i_prevent_my_gel_polish_from_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1l4z30k</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Rainbow Road Nails!!🌈🏎️🏁*credit last pic!!*</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4z30k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1l507vl</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Questions about press-ons</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l507vl/questions_about_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1l506wo</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>What is causing this peeling</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vv63csumrc5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1l506cx</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Suggestions?</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxx8tnzirc5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1l4ynkc</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>I just love green, blue and every shade in between. The first one is my recent nails. I suck at manicure pls ignore that lol.</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4ynkc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1l4zgu9</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Why are electric files used (abused) so much these days?</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l4zgu9/why_are_electric_files_used_abused_so_much_these/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1l4zeva</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Took a risk..</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hax403iwlc5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1l4z73h</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Decided to try a new shape today I usually do square 🥰</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4z73h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1l4z5qw</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>fresh set for Pride 🌈🪩</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yvx14bh2kc5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1l4z28u</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Summer neons!</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0fnbjd9djc5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1l4ysz9</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Acrylic Press Ons By Yours Truly</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4ysz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1l4ypjq</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Any idea what is going on here?</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ae6qtrtgc5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1l4yn2c</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>2 years of doing my own nails (glue on tips &amp; gel)</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lcvdygzbgc5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1l4o7df</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Got new nails</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4o7df</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1l4ql4d</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>waaaay overfiled…what now lol</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4ql4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1l4rjr2</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>My builder gel chipped</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4rjr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1l4uc67</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Accidentally had cuticles trimmed now irritated-at home care?</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4uc67</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1l4tonx</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Nail splits</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l4tonx/nail_splits/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1l4tbnl</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>how to prevent sides of natural nail separating from gel?</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9a9uzrcqdb5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1l4patg</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Can someone explain why my shellac nails lift completely within 1–2 days of application?</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qko09q6jda5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1l4w9b4</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Made this with regular nail polish.</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4w9b4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1l4xcae</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Should I be concerned about this? Got gels for the first time.</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4xcae</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1l4xhad</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Nail routine for a frumpy mom</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l4xhad/nail_routine_for_a_frumpy_mom/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1l4wwkb</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Self made gel nails</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e783ntvt3c5f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1l4woa2</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Looking for a nail tech in London (Chelsea)</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l4woa2/looking_for_a_nail_tech_in_london_chelsea/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1l4w823</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Put on a new suit and go to the wedding</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8kqmmxzwyb5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1l5eztb</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Boyfriend called these 'Modern'</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4126tlg3ig5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1l5e2vo</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Winter's Eve - Inspired Sense</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5e2vo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1l5e1dh</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>I did it!</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jdtqpnfp6g5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1l5dd54</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>best peely base?</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l5dd54/best_peely_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1l5dbda</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Booty call - Jen and Berries (May PPU)</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5dbda</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1l5czej</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Thoughts on Cirque’s new Midsummer collection</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l5czej/thoughts_on_cirques_new_midsummer_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1l5cnzx</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Is it fine for nail salons to shave off the top layer of your nails before gel polish?</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l5cnzx/is_it_fine_for_nail_salons_to_shave_off_the_top/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1l5ci14</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>ILNP Haul</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jem6ea9cpf5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1l5cbmz</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Pompeii Purple, my beloved</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nmywfgmfnf5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1l5c8dc</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Recommendations for polishes with a really strong, glowy, warm pink shimmer?</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l5c8dc/recommendations_for_polishes_with_a_really_strong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1l5c2ru</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Apocalypse Polish haul, swatches, and review!</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5c2ru</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1l5bog6</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Healing nails!! Please help!</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xwq6cm8ogf5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1l5bfs1</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Happy Pride! 🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5bfs1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1l5azdo</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>ILNP Hypnosis is my funky sci-fi dream polish ✨🛸☄️ hard to capture the shift but I’ll try to post a vid on my profile</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5azdo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1l5amxx</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Going to a "Meant To Bee 🐝" themed bridal shower this weekend...</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5amxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1l59hxt</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Cupcake sprinkles🧁</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l59hxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1l59bam</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Am I Everything You Fear?</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avs5bxylte5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1l598eb</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Illusion swatches</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ci6et0iuse5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1l592ac</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Happy Pride! (First attempt at Water Marbling)</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l592ac</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1l58qsr</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>How close is too close….</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l58qsr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1l58hqw</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>New ILNP Magnetic, Hypnosis!</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/RGt3xc4.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1l5892e</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Trying Something New!</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tviyb0fmje5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1l57vs9</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>W7 top coat</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l57vs9/w7_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1l57od7</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Best polishes to get on Etsy?</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l57od7/best_polishes_to_get_on_etsy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1l57m9h</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>🍩 about 2 years late to the trend</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/urw97mvude5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1l57j5p</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Getting back into nail polish! No</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/igz3tvo3de5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1l57fxi</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>1 yr old QoTD 👑 the queen lives</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l57fxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1l57e3s</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Cosmic polish!</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gulrpugvbe5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1l57d1j</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>lapis lazuli inspired nails! 💙</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l57d1j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1l5735v</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Indie recommendations?</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l5735v/indie_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1l56xjf</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Tried the horseshoe + bar magnet trick!</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/otzc0eiw7e5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1l56wee</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>How to swatch thermal polishes?</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l56wee/how_to_swatch_thermal_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1l56urx</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>advice needed for pride tmrw🌈</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l56urx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1l55n7v</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Pear Green Polish with Copper/Gold Shimmer?</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l55n7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1l559na</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>How is Chameleon Nails formula?</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1t7x3bl7ud5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1l557g6</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Choosing Indie Lacquer</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l557g6/choosing_indie_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1l54uoc</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Love is love 🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l54uoc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1l54nrq</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Beaux Rêves have created actual magic!</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l54nrq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1l54hro</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>MC Ribbit Ribbit dupe. dropping tonight at 6pm EST.</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6geh6y55od5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1l5472q</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Shade Names</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/szk0ytyuld5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1l549o3</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Happy Pride!</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l549o3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1l53u28</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Any dupes for this gorgeous (&amp; very much sold out) green?</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/925wb3s1jd5f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1l53rbj</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>11 day wear on the Mango Nails (*not gel* regular nail polish)</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l53rbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1l53pcj</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Neon Skittle - Mooncat and Sally Hansen</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oi130u8vfd5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1l53o9b</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Hard skin around nails</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l53o9b/hard_skin_around_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1l53djc</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Favorite Mooncat dupes?</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l53djc/favorite_mooncat_dupes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1l53bui</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>does it still count as pride if it’s colorful without being rainbow? 😅</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l53bui</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1l52eab</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>This pink is violent, and I love it.</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q2yfigrq7d5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1l52cpq</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>I’m obsessed with pink right now</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l52cpq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1l51pi6</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>shrinkage?</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l51pi6/shrinkage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1l517s8</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>ILNP Flower Child!</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/62yky0s6zc5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1l5159d</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Loved this combo!</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5159d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1l50sre</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Ughh $14 for a drugstore polish?..</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/826rq5z2wc5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1l50r9d</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>New fav thermal 💜</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l50r9d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1l50g5n</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Dupe for OPI Lincoln Park at Midnight</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l50g5n/dupe_for_opi_lincoln_park_at_midnight/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1l5067c</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>My bachlorette nails!</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fq6ac3whrc5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1l5031n</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>A local indie nail polish lover destashed a bunch of her collection and I got it 💅</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5031n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1l4zz22</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Lapis family ring inspired manicure</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4zz22</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1l4zwle</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Glass nail File</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l4zwle/glass_nail_file/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1l4zibh</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>🌈 pride ready for the biggest parade in the world — São Paulo, Brazil</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/menoiitlmc5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1l4zi8v</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Feel like I’m gate-keeping if I don’t share my love for the $4 LA girl “gel” polish!</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4zi8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1l4zee0</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>First Premium Nail Polish Order arrived: ILNP DEEP SPACE 🪐🌌</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4zee0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1l4z9kv</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>🏳️‍🌈OG Gilbert Baker Flag🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4z9kv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1l4z93y</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Blues in loving memory 🩵</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4z93y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1l4z7qf</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Struggle of working with nail polish 😞</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tfk4a3hhkc5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1l4ytsg</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Pink Lady Apple</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4ytsg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1l4ythd</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Barry m</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6bl2s2glhc5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1l4yob4</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Minty fresh</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2ciocxkgc5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1l4ye5l</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Honey Dew Me 🍈</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4ye5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1l4y6cp</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Been having fun with my nails for pride month 🌈💜</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4y6cp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1l4x6o7</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>How long does quick-dry topcoat need to dry before it's safe from bedsheet marks?</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l4x6o7/how_long_does_quickdry_topcoat_need_to_dry_before/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1l4xcr5</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>In love with ILNP Skye 🤩🌌✨</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4xcr5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1l4x0a8</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Playoff Nails (go Oilers!)</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4x0a8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1l4wvzq</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Holo Taco worth gettin?</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l4wvzq/holo_taco_worth_gettin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1l4wc8t</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>on the hunt for oranges</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4wc8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1l4vnpu</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Holo taco Butter Me Up</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zy31ffauub5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1l4vby4</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Polish like Serpents of Eden but without the bright yellow-green?</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4vby4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1l4v6ul</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>First time experiencing shrinkage</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4v6ul</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1l4uuod</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Dandelion sunset nails</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4uuod</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1l4tme7</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Mooncat mixer</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/avwalkmyfb5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1l4p77t</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Professionel gel neglelak brands</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l4p77t/professionel_gel_neglelak_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1l4qhgh</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>i'm a guy and i'm scared</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l4qhgh/im_a_guy_and_im_scared/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1l4sulc</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Happy pride! 🖤 💜🤍💛</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qb68l0z3ab5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1l4sfwn</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Dragon Slay</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4sfwn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1l4s7zc</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>How do indie/boutique cremes compare with drugstore brands you've tried?</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l4s7zc/how_do_indieboutique_cremes_compare_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1l4r7vb</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Throw back to my Halloween nails last year</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oa6bemvmwa5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1l4r17p</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Happy Pride! 🫶🏾🏳️‍⚧️</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4tl5fvxua5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1l5fegj</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>nail art Products</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hsy56gm6ng5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1l5bp95</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Soft girl era 🌸🌸</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/85kuvf9wgf5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1l4l4ks</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Summer Cool Cat Eye Nail Art</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pyanq5cky85f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1l58iyb</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>i started making my own press on nails!</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l58iyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1l5crri</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Try this Butterfly Nails</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ptqo3rrurf5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1l5cqm3</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>New set ✨</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5cqm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1l5cpsv</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Nails in the City</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5cpsv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1l5bn4g</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>What nail art designs do you expect to see offered at a nail salon (besides French and ombre)</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1l5bn4g/what_nail_art_designs_do_you_expect_to_see/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1l5b88a</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Everyone decided to go in very different directions today</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5b88a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1l5b57c</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Frog Nails</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5b57c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1l591jw</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Fresh set of ombré</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ylswd630re5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1l58h90</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Went to a new place.</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2698vkrle5f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1l58e6e</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Another day of making nail stickers on any plastic surface.</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t2zl8idzke5f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1l546fe</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>🌹</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l546fe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1l4zmrv</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>The rhododendron in my front yard inspired this set.</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kcl4d3einc5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1l4z2td</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>A few nail designs my wife has done!</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4z2td</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1l4xyml</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>What tools do you use to get a seamless ombre/gradient design?</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4xyml</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1l4xtxr</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>My first attempt at tortoiseshell.</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mdbg0jckac5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1l4xkri</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/onaj034r8c5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1l4x0fz</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Nail art @isabellanails</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4x0fz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1l4upz3</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Still loving my most recent set - should have had them for valentine's</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xc4eum1ob5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1l4tlk1</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>My own chrome design on my natural nails!</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4tlk1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1l4s3a5</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Just wanted to share my octopus aquarium nail. The blue rings light up under UV light :)</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9de237g14b5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1l4rrj9</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Wifey did these for our vacation</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l4rrj9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1l4rej4</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Forever in love with this teal cat eye 💅✨</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8t74c929ya5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1l4owx0</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Orange vibes⛱️🧡🍊🌼☀️</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwxdleyv8a5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1l4hna6</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Emerald nails 💚</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7onjv8jaz75f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1l3q3es</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Made my bestie some press on nails for a Coldplay concert! ⭐️</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l3q3es</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1l3pfos</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Are these nails are almost snackable? 🍓🍊🍇💅</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rluz4wux415f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1l2y5iy</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>How did I do?</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l2y5iy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1l2ndxf</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Hawaii vibe 💕💅</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qf5nwhug1s4f1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jun  8 08:10:56 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_08.xlsx
+++ b/data/collected_data/2025_06_08.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1350"/>
+  <dimension ref="A1:C1541"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23383,6 +23383,3253 @@
         </is>
       </c>
     </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1l66tqa</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Tips for more natural looking nails + non dominant application</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l66tqa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1l66tfr</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>Galaxy nails 💅🏽 🌌</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3w4w0l2etn5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1l66qjf</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>White nail spots</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mlohw9kesn5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1l66iif</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>I’m so proud of this tiny heart 😭 I had to hold my breath, anchor my feet and pause time itself to do it 💛</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pd8ostpopn5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1l66dd6</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Are these fixable?</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l66dd6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1l65u6y</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>My latest set 🖤</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dswnkznhhn5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1l65jde</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Best nail shape</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l65jde</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1l65cz1</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Rate my nails</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l65cz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1l655ae</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>So jealous of folk whose gel manis last for weeks 😭</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l655ae/so_jealous_of_folk_whose_gel_manis_last_for_weeks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1l654tw</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>How the fuhk does this even happen</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l654tw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1l651qt</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>These came out so well!</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwjqu6c38n5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1l643ul</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>inspo pic vs actual nail art</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l643ul</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1l64yvv</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Cracks on nails? Is this from nail biting?</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l64yvv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1l64rrp</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Pink &amp; green supremacy 🩷💚</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l64rrp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1l649eg</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Rate my nailsss</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9tquns61zm5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1l63vwb</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Rate My Nails!</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iu7vu2lsum5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1l63plw</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>emo lesbian flag nails (self)</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b54t4jpusm5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1l63ebe</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Pride nails as a belated birthday present from my friend. 🏳️‍⚧️🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4zh1j89gpm5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1l631fa</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Fruit Salad 🍑🥝🍓🍍🍊🍋🍉</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oz07j5hmlm5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1l62wo7</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>cunty duckies 😍</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l62wo7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1l62qq0</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Red nails</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l62qq0/red_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1l62lt1</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Super weak damaged nails</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ybtko3z0hm5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1l626l3</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>OPI Nail Envy</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oh4kfp8mcm5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1l625l7</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Just finished my nails</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/449t2k9dcm5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1l5yo6y</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>I've been browsing the nail subs for days for brands/ formulas and just now I purchased Nailtiques Formula 1 based on my nail type</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ygx14hmucl5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1l6011n</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>My favorite sets I did this week! Which one is yours?</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l6011n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1l5zq7q</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>Thoughts about BIAB?</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5zq7q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1l61ffb</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>I don't get my nails done often but wanted something simple and pretty!</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z08mosn25m5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1l617ur</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Builder gel &amp; buggies!</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l617ur</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1l60w8t</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>First time 2 color fill</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4cjqy29vzl5f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1l60qw3</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>French Ombré Stilettos</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgxspn5eyl5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1l60q2a</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l60q2a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1l60ovz</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>Shiny Red</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/laggm9muxl5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1l60ot3</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>White with pops of color</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u6u32hduxl5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1l60ofx</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>PRIDE Mani 2025</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l60ofx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1l607o4</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Butterfly 🦋 Vibes</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l607o4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1l607i1</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Chipped acrylic</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dv7hm6d6tl5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1l5zhw3</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Much gold?</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebj1qlu9ml5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1l5zboz</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Ignore my janky cuticles, but I love what my nail lady did!</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zp6z41hnkl5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1l5z51k</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>UPDATE: On the nails I had no motivation for... I FINALLY FINISHED THEM!!! 🍒💙💓</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5z51k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1l5yv9g</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Subtle lesbian flag nails for pride month</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5yv9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1l5ygji</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>I love it when they ask me for trendy designs 🥹</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ht1tg0fqcl5f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1l5ybbr</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>strawberry pressons</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5ybbr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1l5xzfx</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Just did my nails 🐸🌺💚</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/354a8yej8l5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1l5xuzd</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>My last few sets</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5xuzd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1l5xuhi</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>My First Nail Art!</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5xuhi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1l5xu7n</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>best chrome ever</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5xu7n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1l5xgqm</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Fresh set on point I think!</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u6jxm5204l5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1l5x61i</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>Pride nails</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5x61i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1l5bhqu</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>So, i ripped off my nails.</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2bfzuuiqef5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1l5wmb4</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>Froggie nails!!</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5wmb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1l5wa6n</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>bubble 🫧 POP 🍭 electric</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/98lc9uf2uk5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1l5vuu8</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Honest opinion on these?</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j7kgz9ejqk5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1l5vu9d</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>I told my nail lady to surprise me 🫢</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5vu9d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1l5vg1v</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>After years of being a press-on girl, I’ve officially converted. Dip powder for liiiiife.</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5vg1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1l5v2xm</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Any tips?</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5v2xm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1l5v2xg</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>Happy pride, my bisexual babies 🩷💜💙🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5v2xg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1l5uvgu</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Calling All Gardeners</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l5uvgu/calling_all_gardeners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1l5uuhu</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>I rescued a kitten from the streets last week. I had to match my nails to show off her pretty and unique face pattern 🖤🥹</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5uuhu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1l5ufqc</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Cat eye gems✨</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqhe6bi4fk5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1l5tu63</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>Doing your own nails isn't for the weak 💀💅🏼 It took me 4 hours just to do one hand and now I've lost motivation 🫠</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2jz0li09ak5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1l5tr6m</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Kitty claws</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xwkfyipl9k5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1l5jtvw</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>How damaged are my nails?</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2fvjj9xg2i5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1l5tate</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>1 year without nail biting after doing it my whole life! never thought i’d grow them out, let alone paint them myself and not feel embarrassed. does this color suit my skin tone?</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5tate</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1l5t1e2</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l5t1e2/press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1l5t6hd</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>New summer nails :)</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8l3rt3wz4k5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1l5svs3</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>New nails what do we think?:)</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4v3sncql2k5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1l5sy69</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>Quick opinion… Almond or Coffin for me? I feel I’m too close to be objective…</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5sy69</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1l5spwo</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>How should I shape my natural nails to be less sharp?</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5spwo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1l5sazy</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>I’ve been doing my own manicures with press-ons monthly for two years. 💖</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5sazy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1l5s8me</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time!</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5s8me</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1l5r29h</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>3D Gel Suggestions</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l5r29h/3d_gel_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1l5p4cd</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>First time nails and not happy</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5p4cd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1l5ofoc</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>New design~</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5ofoc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1l5qg6g</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>Please help me find this JR polish colour!</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5qg6g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1l5rap4</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>Top coat changing color?</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jw2nkh89qj5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1l5ryo8</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>Having trouble with gel top coat peeling off</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1l5ryo8/having_trouble_with_gel_top_coat_peeling_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1l5itiz</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>I love these nails 💅</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9c7pmjmcsh5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1l5g69w</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>Did them myself, first time using 3D figures. How do you make them last 3 weeks?</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/adiecxwpwg5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1l5rl9d</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>Feel like a goth cat with these babies</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kil99koisj5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1l5r8u9</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Boho snake</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5r8u9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1l5qc35</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>First time getting nail art</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l6m6onv0jj5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1l5pspm</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>prom nails</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nhr8adlwej5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1l5pp8u</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>Feeling stabby</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5jk57fc6ej5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1l5pct0</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>Experimenting with sparks ✨</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5pct0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1l5p6mo</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>First time doing gel nails and a complicated design on myself</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5p6mo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1l5p1oy</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>ILNP- Hypnosis</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qxjn4zp69j5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1l5okwo</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>When is the most common time to remove acrylic nails?</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8zijic5j5j5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1l5ok5d</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>First acrylic set by myself!</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5ok5d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1l5o4cr</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>A Seche day</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w1i5sgd32j5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1l5ny3e</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>Anyone have any reviews/knowledge on this nail polish?</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8iv3ic7r0j5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1l5nwq2</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>First attempt at watercolor</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b02wws0g0j5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1l5n5nz</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>June Set ♊️</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5n5nz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1l5n18u</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>Eid nails 🎀🤍.</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6vdiltoti5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1l5mih6</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>There is beauty in simplicity, right?</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5mih6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1l5mdg4</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>Island vacation nails! 🏝️</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5mdg4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1l5m8rt</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>Bright pink GelX chrome nails!</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6sc88iteni5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1l5ly4z</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>How did I do?</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wl40u1mzki5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1l5lsi0</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>White gold but for nails 😍💛</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iycg65rpji5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1l5j7ps</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>Safe removal</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5j7ps</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1l660vf</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>Pride swatches</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l660vf/pride_swatches/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1l65wro</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>Fun with magnetics this weekend</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/eul0Vkz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>1l65r4i</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>What are your pride month favorites?</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l65r4i/what_are_your_pride_month_favorites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>1l654of</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>Night Sky Nails</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l654of</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>1l64th0</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>Moody green</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/67pylmic5n5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>1l64p8k</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>Bee's Knees Lacquer's Crabs is Bugs topped with Holo Taco's Everything Taco</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r9zvboqu3n5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>1l64m4q</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>happy pride 🤎🧡🤍🩷❤️</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l64m4q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>1l648o5</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>fishies! 🐟</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l648o5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>1l644w6</t>
+        </is>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>Brat green glitter</t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l644w6/brat_green_glitter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>1l641gn</t>
+        </is>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>Toe beans 💕</t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ey8xy28kwm5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>1l63mdt</t>
+        </is>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>Toasted Marshmallow</t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l63mdt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr">
+        <is>
+          <t>1l62vax</t>
+        </is>
+      </c>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>Rainbow neon mani</t>
+        </is>
+      </c>
+      <c r="C1462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l62vax</t>
+        </is>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr">
+        <is>
+          <t>1l62qhn</t>
+        </is>
+      </c>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>Trans Pride!</t>
+        </is>
+      </c>
+      <c r="C1463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3iw6ve1dim5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr">
+        <is>
+          <t>1l62pd9</t>
+        </is>
+      </c>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>Cracked - Pink Underwing PPU</t>
+        </is>
+      </c>
+      <c r="C1464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l62pd9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr">
+        <is>
+          <t>1l6204m</t>
+        </is>
+      </c>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>Help me find a dupe for Monarch Lacquer’s Petal Dancer</t>
+        </is>
+      </c>
+      <c r="C1465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l6204m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="inlineStr">
+        <is>
+          <t>1l61v6u</t>
+        </is>
+      </c>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t>My The Little Prince polishes came!</t>
+        </is>
+      </c>
+      <c r="C1466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l61v6u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr">
+        <is>
+          <t>1l61gmt</t>
+        </is>
+      </c>
+      <c r="B1467" t="inlineStr">
+        <is>
+          <t>A juicy,jelly sando ft. Wake Up and It’s Showtime and Starburst Reds</t>
+        </is>
+      </c>
+      <c r="C1467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l61gmt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr">
+        <is>
+          <t>1l60nsw</t>
+        </is>
+      </c>
+      <c r="B1468" t="inlineStr">
+        <is>
+          <t>PRIDE Mani 2025</t>
+        </is>
+      </c>
+      <c r="C1468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l60nsw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" t="inlineStr">
+        <is>
+          <t>1l605qw</t>
+        </is>
+      </c>
+      <c r="B1469" t="inlineStr">
+        <is>
+          <t>Essence quick dry top coat</t>
+        </is>
+      </c>
+      <c r="C1469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l605qw/essence_quick_dry_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1470">
+      <c r="A1470" t="inlineStr">
+        <is>
+          <t>1l5zrx1</t>
+        </is>
+      </c>
+      <c r="B1470" t="inlineStr">
+        <is>
+          <t>Sloth Nails</t>
+        </is>
+      </c>
+      <c r="C1470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5zrx1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1471">
+      <c r="A1471" t="inlineStr">
+        <is>
+          <t>1l5zg1z</t>
+        </is>
+      </c>
+      <c r="B1471" t="inlineStr">
+        <is>
+          <t>Koi Whispers and Ribbit Ribbit</t>
+        </is>
+      </c>
+      <c r="C1471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxr8tmgsll5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" t="inlineStr">
+        <is>
+          <t>1l5ypcs</t>
+        </is>
+      </c>
+      <c r="B1472" t="inlineStr">
+        <is>
+          <t>Love this combination ❤️💜</t>
+        </is>
+      </c>
+      <c r="C1472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kcqna3cxel5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1473">
+      <c r="A1473" t="inlineStr">
+        <is>
+          <t>1l5y45x</t>
+        </is>
+      </c>
+      <c r="B1473" t="inlineStr">
+        <is>
+          <t>Yellow Yellow</t>
+        </is>
+      </c>
+      <c r="C1473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5y45x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1474">
+      <c r="A1474" t="inlineStr">
+        <is>
+          <t>1l5xwof</t>
+        </is>
+      </c>
+      <c r="B1474" t="inlineStr">
+        <is>
+          <t>Behold – my latest set! 🤩✨️💕🩵🤍</t>
+        </is>
+      </c>
+      <c r="C1474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6zocf7wv7l5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1475">
+      <c r="A1475" t="inlineStr">
+        <is>
+          <t>1l5xnua</t>
+        </is>
+      </c>
+      <c r="B1475" t="inlineStr">
+        <is>
+          <t>Could someone help explain how to use Cuticula Coconut Milk Sorbet?</t>
+        </is>
+      </c>
+      <c r="C1475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/33k69j1t5l5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1476">
+      <c r="A1476" t="inlineStr">
+        <is>
+          <t>1l5xml5</t>
+        </is>
+      </c>
+      <c r="B1476" t="inlineStr">
+        <is>
+          <t>Cracked - Cordially Invited</t>
+        </is>
+      </c>
+      <c r="C1476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dhdckeui5l5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1477">
+      <c r="A1477" t="inlineStr">
+        <is>
+          <t>1l5xk0w</t>
+        </is>
+      </c>
+      <c r="B1477" t="inlineStr">
+        <is>
+          <t>Camera-breaker aka 90s inflatable furniture</t>
+        </is>
+      </c>
+      <c r="C1477" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dj3odbow4l5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1478">
+      <c r="A1478" t="inlineStr">
+        <is>
+          <t>1l5xd5j</t>
+        </is>
+      </c>
+      <c r="B1478" t="inlineStr">
+        <is>
+          <t>What nail shape is this?</t>
+        </is>
+      </c>
+      <c r="C1478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5xd5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1479">
+      <c r="A1479" t="inlineStr">
+        <is>
+          <t>1l5x93d</t>
+        </is>
+      </c>
+      <c r="B1479" t="inlineStr">
+        <is>
+          <t>In DC for the weekend wearing Forces of Evil.</t>
+        </is>
+      </c>
+      <c r="C1479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1lctlfb2l5f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1480">
+      <c r="A1480" t="inlineStr">
+        <is>
+          <t>1l5x3py</t>
+        </is>
+      </c>
+      <c r="B1480" t="inlineStr">
+        <is>
+          <t>A little melted moment 🫠🍥🌀</t>
+        </is>
+      </c>
+      <c r="C1480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n7uho6911l5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1481">
+      <c r="A1481" t="inlineStr">
+        <is>
+          <t>1l5wim0</t>
+        </is>
+      </c>
+      <c r="B1481" t="inlineStr">
+        <is>
+          <t>First time trying nail wraps</t>
+        </is>
+      </c>
+      <c r="C1481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ad0jfvv0wk5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1482">
+      <c r="A1482" t="inlineStr">
+        <is>
+          <t>1l5whi7</t>
+        </is>
+      </c>
+      <c r="B1482" t="inlineStr">
+        <is>
+          <t>👽💜🛸</t>
+        </is>
+      </c>
+      <c r="C1482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5whi7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1483">
+      <c r="A1483" t="inlineStr">
+        <is>
+          <t>1l5whi4</t>
+        </is>
+      </c>
+      <c r="B1483" t="inlineStr">
+        <is>
+          <t>Queen of the Dead</t>
+        </is>
+      </c>
+      <c r="C1483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5whi4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1484">
+      <c r="A1484" t="inlineStr">
+        <is>
+          <t>1l5wfmh</t>
+        </is>
+      </c>
+      <c r="B1484" t="inlineStr">
+        <is>
+          <t>My alien nails for a festival coming up !</t>
+        </is>
+      </c>
+      <c r="C1484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5wfmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1485">
+      <c r="A1485" t="inlineStr">
+        <is>
+          <t>1l5wb8h</t>
+        </is>
+      </c>
+      <c r="B1485" t="inlineStr">
+        <is>
+          <t>my first ilnp order! can you guess my favorite seasonal color scheme lol</t>
+        </is>
+      </c>
+      <c r="C1485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5wb8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1486">
+      <c r="A1486" t="inlineStr">
+        <is>
+          <t>1l5w65m</t>
+        </is>
+      </c>
+      <c r="B1486" t="inlineStr">
+        <is>
+          <t>Accidental exact match! (Plus a bonus match!)</t>
+        </is>
+      </c>
+      <c r="C1486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5w65m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1487">
+      <c r="A1487" t="inlineStr">
+        <is>
+          <t>1l5veml</t>
+        </is>
+      </c>
+      <c r="B1487" t="inlineStr">
+        <is>
+          <t>Fiery Attraction 🥵</t>
+        </is>
+      </c>
+      <c r="C1487" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ko2lulx4mk5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1488">
+      <c r="A1488" t="inlineStr">
+        <is>
+          <t>1l5uxev</t>
+        </is>
+      </c>
+      <c r="B1488" t="inlineStr">
+        <is>
+          <t>Normally hate neons</t>
+        </is>
+      </c>
+      <c r="C1488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5uxev</t>
+        </is>
+      </c>
+    </row>
+    <row r="1489">
+      <c r="A1489" t="inlineStr">
+        <is>
+          <t>1l5uusv</t>
+        </is>
+      </c>
+      <c r="B1489" t="inlineStr">
+        <is>
+          <t>happy pride y’all! 🌈</t>
+        </is>
+      </c>
+      <c r="C1489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5uusv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1490">
+      <c r="A1490" t="inlineStr">
+        <is>
+          <t>1l5ur73</t>
+        </is>
+      </c>
+      <c r="B1490" t="inlineStr">
+        <is>
+          <t>Nail glue over polish</t>
+        </is>
+      </c>
+      <c r="C1490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l5ur73/nail_glue_over_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1491">
+      <c r="A1491" t="inlineStr">
+        <is>
+          <t>1l5uhwk</t>
+        </is>
+      </c>
+      <c r="B1491" t="inlineStr">
+        <is>
+          <t>A Juicy Rainbow Skittle Jelly Sandwich</t>
+        </is>
+      </c>
+      <c r="C1491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5uhwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1492">
+      <c r="A1492" t="inlineStr">
+        <is>
+          <t>1l5uhi1</t>
+        </is>
+      </c>
+      <c r="B1492" t="inlineStr">
+        <is>
+          <t>Polish with the longest name I’ve owned</t>
+        </is>
+      </c>
+      <c r="C1492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5uhi1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1493">
+      <c r="A1493" t="inlineStr">
+        <is>
+          <t>1l5svln</t>
+        </is>
+      </c>
+      <c r="B1493" t="inlineStr">
+        <is>
+          <t>Birthday / Pride Month ft HT Retro Collection</t>
+        </is>
+      </c>
+      <c r="C1493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5svln</t>
+        </is>
+      </c>
+    </row>
+    <row r="1494">
+      <c r="A1494" t="inlineStr">
+        <is>
+          <t>1l5spt3</t>
+        </is>
+      </c>
+      <c r="B1494" t="inlineStr">
+        <is>
+          <t>My first gel set</t>
+        </is>
+      </c>
+      <c r="C1494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d61c14z81k5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1495">
+      <c r="A1495" t="inlineStr">
+        <is>
+          <t>1l5qmgm</t>
+        </is>
+      </c>
+      <c r="B1495" t="inlineStr">
+        <is>
+          <t>obligatory pride nails</t>
+        </is>
+      </c>
+      <c r="C1495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kt6zu7u6lj5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1496">
+      <c r="A1496" t="inlineStr">
+        <is>
+          <t>1l5s84z</t>
+        </is>
+      </c>
+      <c r="B1496" t="inlineStr">
+        <is>
+          <t>Pride nails but make them pink 🌈🎀</t>
+        </is>
+      </c>
+      <c r="C1496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5s84z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1497">
+      <c r="A1497" t="inlineStr">
+        <is>
+          <t>1l5s1ll</t>
+        </is>
+      </c>
+      <c r="B1497" t="inlineStr">
+        <is>
+          <t>Would 2 base coats work together?</t>
+        </is>
+      </c>
+      <c r="C1497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l5s1ll/would_2_base_coats_work_together/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1498">
+      <c r="A1498" t="inlineStr">
+        <is>
+          <t>1l5rid2</t>
+        </is>
+      </c>
+      <c r="B1498" t="inlineStr">
+        <is>
+          <t>Looking for a brand that has unique magnetic polishes</t>
+        </is>
+      </c>
+      <c r="C1498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l5rid2/looking_for_a_brand_that_has_unique_magnetic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1499">
+      <c r="A1499" t="inlineStr">
+        <is>
+          <t>1l5rehx</t>
+        </is>
+      </c>
+      <c r="B1499" t="inlineStr">
+        <is>
+          <t>dupe request! "Nina Ultra Pro: Passion Pink" (709230)</t>
+        </is>
+      </c>
+      <c r="C1499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5rehx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1500">
+      <c r="A1500" t="inlineStr">
+        <is>
+          <t>1l5rbc8</t>
+        </is>
+      </c>
+      <c r="B1500" t="inlineStr">
+        <is>
+          <t>A rainbow gradient? For pride? Groundbreaking.</t>
+        </is>
+      </c>
+      <c r="C1500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5rbc8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1501">
+      <c r="A1501" t="inlineStr">
+        <is>
+          <t>1l5r929</t>
+        </is>
+      </c>
+      <c r="B1501" t="inlineStr">
+        <is>
+          <t>LA Colors Hyperactive &amp; Headliner</t>
+        </is>
+      </c>
+      <c r="C1501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aooyxflwpj5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1502">
+      <c r="A1502" t="inlineStr">
+        <is>
+          <t>1l5qvfl</t>
+        </is>
+      </c>
+      <c r="B1502" t="inlineStr">
+        <is>
+          <t>Polish that is a sheer/jelly/milky *cool tone* white?</t>
+        </is>
+      </c>
+      <c r="C1502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l5qvfl/polish_that_is_a_sheerjellymilky_cool_tone_white/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1503">
+      <c r="A1503" t="inlineStr">
+        <is>
+          <t>1l5qoqy</t>
+        </is>
+      </c>
+      <c r="B1503" t="inlineStr">
+        <is>
+          <t>Strengtheners on already strong nails</t>
+        </is>
+      </c>
+      <c r="C1503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l5qoqy/strengtheners_on_already_strong_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1504">
+      <c r="A1504" t="inlineStr">
+        <is>
+          <t>1l5py54</t>
+        </is>
+      </c>
+      <c r="B1504" t="inlineStr">
+        <is>
+          <t>Can’t Stop Looking 🤩</t>
+        </is>
+      </c>
+      <c r="C1504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z16ck7g2gj5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1505">
+      <c r="A1505" t="inlineStr">
+        <is>
+          <t>1l5pvih</t>
+        </is>
+      </c>
+      <c r="B1505" t="inlineStr">
+        <is>
+          <t>Will Chamaeleon restock the Wonderful Worlds collection?</t>
+        </is>
+      </c>
+      <c r="C1505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l5pvih/will_chamaeleon_restock_the_wonderful_worlds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1506">
+      <c r="A1506" t="inlineStr">
+        <is>
+          <t>1l5ple0</t>
+        </is>
+      </c>
+      <c r="B1506" t="inlineStr">
+        <is>
+          <t>Red Wine Supernova - Pahlish</t>
+        </is>
+      </c>
+      <c r="C1506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5ple0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1507">
+      <c r="A1507" t="inlineStr">
+        <is>
+          <t>1l5p5km</t>
+        </is>
+      </c>
+      <c r="B1507" t="inlineStr">
+        <is>
+          <t>Cracked - 23 Flavors</t>
+        </is>
+      </c>
+      <c r="C1507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5p5km</t>
+        </is>
+      </c>
+    </row>
+    <row r="1508">
+      <c r="A1508" t="inlineStr">
+        <is>
+          <t>1l5p1t3</t>
+        </is>
+      </c>
+      <c r="B1508" t="inlineStr">
+        <is>
+          <t>My first jelly sammie</t>
+        </is>
+      </c>
+      <c r="C1508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5p1t3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1509">
+      <c r="A1509" t="inlineStr">
+        <is>
+          <t>1l5oybh</t>
+        </is>
+      </c>
+      <c r="B1509" t="inlineStr">
+        <is>
+          <t>Question: what’s the best true blue red (cool toned red) polish according to you?</t>
+        </is>
+      </c>
+      <c r="C1509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l5oybh/question_whats_the_best_true_blue_red_cool_toned/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1510">
+      <c r="A1510" t="inlineStr">
+        <is>
+          <t>1l5olu6</t>
+        </is>
+      </c>
+      <c r="B1510" t="inlineStr">
+        <is>
+          <t>Phoenix indie: Sabrewing hummingbird</t>
+        </is>
+      </c>
+      <c r="C1510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5olu6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1511">
+      <c r="A1511" t="inlineStr">
+        <is>
+          <t>1l5odb4</t>
+        </is>
+      </c>
+      <c r="B1511" t="inlineStr">
+        <is>
+          <t>Londontown Chai</t>
+        </is>
+      </c>
+      <c r="C1511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5odb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1512">
+      <c r="A1512" t="inlineStr">
+        <is>
+          <t>1l5obl1</t>
+        </is>
+      </c>
+      <c r="B1512" t="inlineStr">
+        <is>
+          <t>Anyone else falling out of love with Zoya? They are so so stagnant and behind the times</t>
+        </is>
+      </c>
+      <c r="C1512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l5obl1/anyone_else_falling_out_of_love_with_zoya_they/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1513">
+      <c r="A1513" t="inlineStr">
+        <is>
+          <t>1l5o4lh</t>
+        </is>
+      </c>
+      <c r="B1513" t="inlineStr">
+        <is>
+          <t>A surprise House of Hades dupe…loving this brilliant blue!</t>
+        </is>
+      </c>
+      <c r="C1513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5o4lh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1514">
+      <c r="A1514" t="inlineStr">
+        <is>
+          <t>1l5n7l8</t>
+        </is>
+      </c>
+      <c r="B1514" t="inlineStr">
+        <is>
+          <t>I had to file my nails short again, but at least I still have cute polish ✨</t>
+        </is>
+      </c>
+      <c r="C1514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5fj96he0vi5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1515">
+      <c r="A1515" t="inlineStr">
+        <is>
+          <t>1l5n3qu</t>
+        </is>
+      </c>
+      <c r="B1515" t="inlineStr">
+        <is>
+          <t>An open discussion about self-promotion, rule 5, and flair (both user and post)</t>
+        </is>
+      </c>
+      <c r="C1515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l5n3qu/an_open_discussion_about_selfpromotion_rule_5_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1516">
+      <c r="A1516" t="inlineStr">
+        <is>
+          <t>1l5n34b</t>
+        </is>
+      </c>
+      <c r="B1516" t="inlineStr">
+        <is>
+          <t>Nail Tek vs Nailtiques?</t>
+        </is>
+      </c>
+      <c r="C1516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l5n34b/nail_tek_vs_nailtiques/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1517">
+      <c r="A1517" t="inlineStr">
+        <is>
+          <t>1l5mml1</t>
+        </is>
+      </c>
+      <c r="B1517" t="inlineStr">
+        <is>
+          <t>🏳️‍🌈💚Gay/MLM Pride Flag💙🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5mml1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1518">
+      <c r="A1518" t="inlineStr">
+        <is>
+          <t>1l5lz97</t>
+        </is>
+      </c>
+      <c r="B1518" t="inlineStr">
+        <is>
+          <t>Pride inspired abstract set</t>
+        </is>
+      </c>
+      <c r="C1518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5lz97</t>
+        </is>
+      </c>
+    </row>
+    <row r="1519">
+      <c r="A1519" t="inlineStr">
+        <is>
+          <t>1l5lurg</t>
+        </is>
+      </c>
+      <c r="B1519" t="inlineStr">
+        <is>
+          <t>Mesmerized by Deep Space 😍</t>
+        </is>
+      </c>
+      <c r="C1519" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8hs3hi28ki5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1520">
+      <c r="A1520" t="inlineStr">
+        <is>
+          <t>1l5lrc5</t>
+        </is>
+      </c>
+      <c r="B1520" t="inlineStr">
+        <is>
+          <t>Pride Month Nails 🌈</t>
+        </is>
+      </c>
+      <c r="C1520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5lrc5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1521">
+      <c r="A1521" t="inlineStr">
+        <is>
+          <t>1l5knuv</t>
+        </is>
+      </c>
+      <c r="B1521" t="inlineStr">
+        <is>
+          <t>When the mid-mani topper hits just right 🤌</t>
+        </is>
+      </c>
+      <c r="C1521" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lq7rqy4y9i5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1522">
+      <c r="A1522" t="inlineStr">
+        <is>
+          <t>1l5kkmr</t>
+        </is>
+      </c>
+      <c r="B1522" t="inlineStr">
+        <is>
+          <t>For those who wear gel top coat over regular nail polish, how long does it last?</t>
+        </is>
+      </c>
+      <c r="C1522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l5kkmr/for_those_who_wear_gel_top_coat_over_regular_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1523">
+      <c r="A1523" t="inlineStr">
+        <is>
+          <t>1l5kd3k</t>
+        </is>
+      </c>
+      <c r="B1523" t="inlineStr">
+        <is>
+          <t>Dupes?</t>
+        </is>
+      </c>
+      <c r="C1523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/azqgmcqd7i5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1524">
+      <c r="A1524" t="inlineStr">
+        <is>
+          <t>1l5j4zz</t>
+        </is>
+      </c>
+      <c r="B1524" t="inlineStr">
+        <is>
+          <t>Ridge filling base coat</t>
+        </is>
+      </c>
+      <c r="C1524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l5j4zz/ridge_filling_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1525">
+      <c r="A1525" t="inlineStr">
+        <is>
+          <t>1l5hvz2</t>
+        </is>
+      </c>
+      <c r="B1525" t="inlineStr">
+        <is>
+          <t>Desert Island Nail Polish 🏝️: You Can Only Pick 3! What Are Your Lifers?</t>
+        </is>
+      </c>
+      <c r="C1525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l5hvz2/desert_island_nail_polish_you_can_only_pick_3/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1526">
+      <c r="A1526" t="inlineStr">
+        <is>
+          <t>1l5g0w2</t>
+        </is>
+      </c>
+      <c r="B1526" t="inlineStr">
+        <is>
+          <t>Help me find a 2000's or 2010's confetti nail polish!</t>
+        </is>
+      </c>
+      <c r="C1526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1l5g0w2/help_me_find_a_2000s_or_2010s_confetti_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1527">
+      <c r="A1527" t="inlineStr">
+        <is>
+          <t>1l62lq4</t>
+        </is>
+      </c>
+      <c r="B1527" t="inlineStr">
+        <is>
+          <t>Incapsulated dried flowers on my nails 🥰</t>
+        </is>
+      </c>
+      <c r="C1527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vagxqdyzgm5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1528">
+      <c r="A1528" t="inlineStr">
+        <is>
+          <t>1l63zkn</t>
+        </is>
+      </c>
+      <c r="B1528" t="inlineStr">
+        <is>
+          <t>This Cat eye is too cute 🥹 I finally tried it on a client.</t>
+        </is>
+      </c>
+      <c r="C1528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tuwmg3lyvm5f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1529">
+      <c r="A1529" t="inlineStr">
+        <is>
+          <t>1l63nqv</t>
+        </is>
+      </c>
+      <c r="B1529" t="inlineStr">
+        <is>
+          <t>How did they turn out for me?</t>
+        </is>
+      </c>
+      <c r="C1529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q92kua6asm5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1530">
+      <c r="A1530" t="inlineStr">
+        <is>
+          <t>1l60a77</t>
+        </is>
+      </c>
+      <c r="B1530" t="inlineStr">
+        <is>
+          <t>My nails today, how do you think?</t>
+        </is>
+      </c>
+      <c r="C1530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l21vqzovtl5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1531">
+      <c r="A1531" t="inlineStr">
+        <is>
+          <t>1l5z1v4</t>
+        </is>
+      </c>
+      <c r="B1531" t="inlineStr">
+        <is>
+          <t>First try with gel</t>
+        </is>
+      </c>
+      <c r="C1531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5z1v4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1532">
+      <c r="A1532" t="inlineStr">
+        <is>
+          <t>1l5yxe6</t>
+        </is>
+      </c>
+      <c r="B1532" t="inlineStr">
+        <is>
+          <t>DIY manicure I did at home</t>
+        </is>
+      </c>
+      <c r="C1532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2si6ddgigl5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1533">
+      <c r="A1533" t="inlineStr">
+        <is>
+          <t>1l5xeqw</t>
+        </is>
+      </c>
+      <c r="B1533" t="inlineStr">
+        <is>
+          <t>My pride nails!</t>
+        </is>
+      </c>
+      <c r="C1533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fkpx3h2o3l5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1534">
+      <c r="A1534" t="inlineStr">
+        <is>
+          <t>1l5r65q</t>
+        </is>
+      </c>
+      <c r="B1534" t="inlineStr">
+        <is>
+          <t>Boho snake</t>
+        </is>
+      </c>
+      <c r="C1534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5r65q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1535">
+      <c r="A1535" t="inlineStr">
+        <is>
+          <t>1l5qxmr</t>
+        </is>
+      </c>
+      <c r="B1535" t="inlineStr">
+        <is>
+          <t>Pride nails done by me, pt 2</t>
+        </is>
+      </c>
+      <c r="C1535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f6uoxt0jnj5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1536">
+      <c r="A1536" t="inlineStr">
+        <is>
+          <t>1l5py0i</t>
+        </is>
+      </c>
+      <c r="B1536" t="inlineStr">
+        <is>
+          <t>Happy National Donut Day… yesterday!</t>
+        </is>
+      </c>
+      <c r="C1536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5py0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1537">
+      <c r="A1537" t="inlineStr">
+        <is>
+          <t>1l5nvra</t>
+        </is>
+      </c>
+      <c r="B1537" t="inlineStr">
+        <is>
+          <t>Handpainted on myself for Bali vacation 💙🤎</t>
+        </is>
+      </c>
+      <c r="C1537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5nvra</t>
+        </is>
+      </c>
+    </row>
+    <row r="1538">
+      <c r="A1538" t="inlineStr">
+        <is>
+          <t>1l5lzi0</t>
+        </is>
+      </c>
+      <c r="B1538" t="inlineStr">
+        <is>
+          <t>How do you decide on what fingers to do what design?</t>
+        </is>
+      </c>
+      <c r="C1538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1l5lzi0/how_do_you_decide_on_what_fingers_to_do_what/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1539">
+      <c r="A1539" t="inlineStr">
+        <is>
+          <t>1l5lqw4</t>
+        </is>
+      </c>
+      <c r="B1539" t="inlineStr">
+        <is>
+          <t>Can’t help but look for a fairy 🧚‍♀️</t>
+        </is>
+      </c>
+      <c r="C1539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yovf2tecji5f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1540">
+      <c r="A1540" t="inlineStr">
+        <is>
+          <t>1l5jgfn</t>
+        </is>
+      </c>
+      <c r="B1540" t="inlineStr">
+        <is>
+          <t>Rainbow 🌈 lazy gradient</t>
+        </is>
+      </c>
+      <c r="C1540" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p8cbgiouyh5f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1541">
+      <c r="A1541" t="inlineStr">
+        <is>
+          <t>1l5iog7</t>
+        </is>
+      </c>
+      <c r="B1541" t="inlineStr">
+        <is>
+          <t>Recent nail art I’ve done 💅</t>
+        </is>
+      </c>
+      <c r="C1541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1l5iog7</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>